<commit_message>
Fixes from teacher + checkstyle + speed tests (unsuccessful)
</commit_message>
<xml_diff>
--- a/Task_2_1_1/time.xlsx
+++ b/Task_2_1_1/time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\NSU\OOP\Task_2_1_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7030909D-594D-4EA6-AD7D-ABCAE01B5FDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE64AC8F-EB5A-4CE8-B07F-BD227DAD8706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D5ABC52E-7C61-45CD-9E16-B81EF21C7B9D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D5ABC52E-7C61-45CD-9E16-B81EF21C7B9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>Usual</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>arr.length = 1kk</t>
+  </si>
+  <si>
+    <t>с 10-кратным повторением (поделил на 10 потом)</t>
   </si>
 </sst>
 </file>
@@ -90,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +124,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -135,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -146,6 +155,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -375,103 +387,103 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>28.433299999999999</c:v>
+                  <c:v>33.545449999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.979399999999998</c:v>
+                  <c:v>102.09437333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.539000000000001</c:v>
+                  <c:v>31.84225</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>244.04139999999998</c:v>
+                  <c:v>286.87023999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>357.42309999999998</c:v>
+                  <c:v>354.46147333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>345.21359999999999</c:v>
+                  <c:v>377.6347566666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>409.80440000000004</c:v>
+                  <c:v>433.45422333333335</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>430.00529999999998</c:v>
+                  <c:v>437.4499633333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>361.16929999999996</c:v>
+                  <c:v>410.13909666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>356.28479999999996</c:v>
+                  <c:v>403.21022999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>373.30279999999999</c:v>
+                  <c:v>422.72969333333327</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>366.31540000000001</c:v>
+                  <c:v>408.34453999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>328.73090000000002</c:v>
+                  <c:v>382.1543733333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>332.58629999999999</c:v>
+                  <c:v>373.7577766666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>316.14259999999996</c:v>
+                  <c:v>349.93829333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>329.6748</c:v>
+                  <c:v>349.15191666666669</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>311.63069999999999</c:v>
+                  <c:v>334.30834999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>304.33800000000002</c:v>
+                  <c:v>320.80375666666669</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>316.92399999999998</c:v>
+                  <c:v>330.76777000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>300.46609999999998</c:v>
+                  <c:v>329.44851</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>303.16070000000002</c:v>
+                  <c:v>318.64961999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>297.2799</c:v>
+                  <c:v>316.99907000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>304.0249</c:v>
+                  <c:v>313.93516999999997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>302.67720000000003</c:v>
+                  <c:v>326.15464666666668</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>297.9658</c:v>
+                  <c:v>317.04913666666664</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>309.1771</c:v>
+                  <c:v>322.84330666666671</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>303.77499999999998</c:v>
+                  <c:v>362.56063666666665</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>313.49650000000003</c:v>
+                  <c:v>327.00149333333331</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>299.80829999999997</c:v>
+                  <c:v>318.19207333333333</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>313.28709999999995</c:v>
+                  <c:v>328.18165000000005</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>304.2038</c:v>
+                  <c:v>360.72090999999995</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>306.58709999999996</c:v>
+                  <c:v>360.95258000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>304.6198</c:v>
+                  <c:v>342.80452000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -857,103 +869,103 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>212.6105</c:v>
+                  <c:v>213.75745000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>269.43540000000002</c:v>
+                  <c:v>968.4126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>235.7038</c:v>
+                  <c:v>220.41729999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2504.6324</c:v>
+                  <c:v>2520.1049750000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3336.4681</c:v>
+                  <c:v>3125.7725</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4147.0815000000002</c:v>
+                  <c:v>3732.9300750000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4164.6562000000004</c:v>
+                  <c:v>3659.3316500000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4052.0135</c:v>
+                  <c:v>3422.7775499999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3544.3163999999997</c:v>
+                  <c:v>3099.3313750000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3630.1227999999996</c:v>
+                  <c:v>3121.9437749999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3661.4503999999997</c:v>
+                  <c:v>3171.8808749999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3592.1977000000002</c:v>
+                  <c:v>3155.7731749999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3378.9196000000002</c:v>
+                  <c:v>3163.0625249999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3440.2542000000003</c:v>
+                  <c:v>3258.3580499999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4122.3252999999995</c:v>
+                  <c:v>3264.6103499999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4121.1535999999996</c:v>
+                  <c:v>3187.1091499999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4722.8922000000002</c:v>
+                  <c:v>3352.389525</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4327.9656999999997</c:v>
+                  <c:v>3198.14455</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4230.5754999999999</c:v>
+                  <c:v>3168.8187749999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4175.8537000000006</c:v>
+                  <c:v>3163.9285249999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4119.384</c:v>
+                  <c:v>3142.725375</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4490.6172999999999</c:v>
+                  <c:v>3241.3328999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4326.2375999999995</c:v>
+                  <c:v>3198.67355</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4635.0565999999999</c:v>
+                  <c:v>3290.8587000000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4084.4297999999999</c:v>
+                  <c:v>3143.5763999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2444.9911000000002</c:v>
+                  <c:v>2768.4515499999998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1654.5496000000001</c:v>
+                  <c:v>2509.0195750000003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1788.7021000000002</c:v>
+                  <c:v>2572.3301749999996</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2013.2529</c:v>
+                  <c:v>2580.5604500000004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2199.1061</c:v>
+                  <c:v>2763.2431499999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3448.3698999999997</c:v>
+                  <c:v>3042.1008500000003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4435.7227000000003</c:v>
+                  <c:v>3287.0614500000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4172.9618</c:v>
+                  <c:v>3291.7092000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1343,103 +1355,103 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>9.5226000000000006</c:v>
+                  <c:v>23.286999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.0075</c:v>
+                  <c:v>35.515500000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5449999999999999</c:v>
+                  <c:v>17.363849999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.907400000000003</c:v>
+                  <c:v>45.317999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.357700000000001</c:v>
+                  <c:v>52.698250000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.192400000000003</c:v>
+                  <c:v>41.61795</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.198499999999999</c:v>
+                  <c:v>43.782249999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.6312</c:v>
+                  <c:v>41.986050000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.214299999999998</c:v>
+                  <c:v>42.423250000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26.324999999999999</c:v>
+                  <c:v>43.198250000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28.3794</c:v>
+                  <c:v>37.142400000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.309200000000001</c:v>
+                  <c:v>40.909550000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25.7515</c:v>
+                  <c:v>36.543550000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.646699999999999</c:v>
+                  <c:v>36.555199999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.866299999999999</c:v>
+                  <c:v>36.462449999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.5045</c:v>
+                  <c:v>34.431650000000005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22.041499999999999</c:v>
+                  <c:v>33.344149999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.369299999999999</c:v>
+                  <c:v>32.16545</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22.180900000000001</c:v>
+                  <c:v>32.469349999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21.127299999999998</c:v>
+                  <c:v>33.022150000000003</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23.638000000000002</c:v>
+                  <c:v>33.774149999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23.418700000000001</c:v>
+                  <c:v>32.425849999999997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.867599999999999</c:v>
+                  <c:v>33.772599999999997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.659400000000002</c:v>
+                  <c:v>35.000599999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23.844000000000001</c:v>
+                  <c:v>34.5334</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>22.4389</c:v>
+                  <c:v>34.182250000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>23.099900000000002</c:v>
+                  <c:v>32.964150000000004</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>21.9511</c:v>
+                  <c:v>35.02225</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>21.07</c:v>
+                  <c:v>33.097749999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>23.7775</c:v>
+                  <c:v>32.353650000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>20.517900000000001</c:v>
+                  <c:v>33.407849999999996</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>19.984900000000003</c:v>
+                  <c:v>30.833200000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>21.168400000000002</c:v>
+                  <c:v>31.266349999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3255,16 +3267,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>17369</xdr:rowOff>
+      <xdr:rowOff>4669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>361951</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>463551</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>51547</xdr:rowOff>
+      <xdr:rowOff>38847</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3291,14 +3303,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>86332</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>22832</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>65748</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>168088</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>104588</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>85187</xdr:rowOff>
     </xdr:to>
@@ -3327,16 +3339,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>69848</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>44448</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>82548</xdr:rowOff>
+      <xdr:rowOff>184148</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>469899</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>63499</xdr:rowOff>
+      <xdr:rowOff>165099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3661,10 +3673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D94D687-82E9-4018-8178-D13A8669E2BA}">
-  <dimension ref="B2:AB109"/>
+  <dimension ref="B2:AG147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AA38" sqref="AA38"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,6 +3684,7 @@
     <col min="2" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="8" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3685,30 +3698,62 @@
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5">
-        <f>E3 / 1000 / 1000</f>
-        <v>9.5226000000000006</v>
-      </c>
-      <c r="E3">
-        <v>9522600</v>
-      </c>
+      <c r="D3" s="10">
+        <f>SUM(E3:N3) / COUNT(E3:N3)/ 1000 / 1000</f>
+        <v>23.286999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>23847200</v>
+      </c>
+      <c r="F3" s="1">
+        <v>22726800</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5">
-        <f t="shared" ref="D4:D35" si="0">E4 / 1000 / 1000</f>
-        <v>12.0075</v>
-      </c>
-      <c r="E4">
-        <v>12007500</v>
-      </c>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:D35" si="0">SUM(E4:N4) / COUNT(E4:N4)/ 1000 / 1000</f>
+        <v>35.515500000000003</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43068800</v>
+      </c>
+      <c r="F4" s="1">
+        <v>27962200</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -3717,39 +3762,72 @@
       <c r="C5" s="7">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>9.5449999999999999</v>
-      </c>
-      <c r="E5">
-        <v>9545000</v>
-      </c>
+        <v>17.363849999999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>17070500</v>
+      </c>
+      <c r="F5" s="1">
+        <v>17657200</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="7">
         <v>2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="10">
         <f t="shared" si="0"/>
-        <v>35.907400000000003</v>
-      </c>
-      <c r="E6">
-        <v>35907400</v>
-      </c>
+        <v>45.317999999999998</v>
+      </c>
+      <c r="E6" s="1">
+        <v>34034800</v>
+      </c>
+      <c r="F6" s="1">
+        <v>56601200</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="7">
         <v>3</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="10">
         <f t="shared" si="0"/>
-        <v>29.357700000000001</v>
-      </c>
-      <c r="E7">
-        <v>29357700</v>
-      </c>
+        <v>52.698250000000002</v>
+      </c>
+      <c r="E7" s="1">
+        <v>55877500</v>
+      </c>
+      <c r="F7" s="1">
+        <v>49519000</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
       <c r="AB7" s="8"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
@@ -3757,13 +3835,24 @@
       <c r="C8" s="7">
         <v>4</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="10">
         <f t="shared" si="0"/>
-        <v>31.192400000000003</v>
-      </c>
-      <c r="E8">
-        <v>31192400</v>
-      </c>
+        <v>41.61795</v>
+      </c>
+      <c r="E8" s="1">
+        <v>38368400</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44867500</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
       <c r="AB8" s="8"/>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
@@ -3771,13 +3860,24 @@
       <c r="C9" s="7">
         <v>5</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="10">
         <f t="shared" si="0"/>
-        <v>31.198499999999999</v>
-      </c>
-      <c r="E9">
-        <v>31198500</v>
-      </c>
+        <v>43.782249999999998</v>
+      </c>
+      <c r="E9" s="1">
+        <v>42445500</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45119000</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
       <c r="AB9" s="8"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
@@ -3785,13 +3885,24 @@
       <c r="C10" s="7">
         <v>6</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="10">
         <f t="shared" si="0"/>
-        <v>28.6312</v>
-      </c>
-      <c r="E10">
-        <v>28631200</v>
-      </c>
+        <v>41.986050000000006</v>
+      </c>
+      <c r="E10" s="1">
+        <v>43871300</v>
+      </c>
+      <c r="F10" s="1">
+        <v>40100800</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
       <c r="AB10" s="8"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
@@ -3799,13 +3910,24 @@
       <c r="C11" s="7">
         <v>7</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="10">
         <f t="shared" si="0"/>
-        <v>28.214299999999998</v>
-      </c>
-      <c r="E11">
-        <v>28214300</v>
-      </c>
+        <v>42.423250000000003</v>
+      </c>
+      <c r="E11" s="1">
+        <v>41498800</v>
+      </c>
+      <c r="F11" s="1">
+        <v>43347700</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
       <c r="AB11" s="8"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
@@ -3813,13 +3935,24 @@
       <c r="C12" s="7">
         <v>8</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="10">
         <f t="shared" si="0"/>
-        <v>26.324999999999999</v>
-      </c>
-      <c r="E12">
-        <v>26325000</v>
-      </c>
+        <v>43.198250000000002</v>
+      </c>
+      <c r="E12" s="1">
+        <v>42146400</v>
+      </c>
+      <c r="F12" s="1">
+        <v>44250100</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
       <c r="AB12" s="8"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
@@ -3827,13 +3960,24 @@
       <c r="C13" s="7">
         <v>9</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>28.3794</v>
-      </c>
-      <c r="E13">
-        <v>28379400</v>
-      </c>
+        <v>37.142400000000002</v>
+      </c>
+      <c r="E13" s="1">
+        <v>38486800</v>
+      </c>
+      <c r="F13" s="1">
+        <v>35798000</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
       <c r="AB13" s="8"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
@@ -3841,13 +3985,24 @@
       <c r="C14" s="7">
         <v>10</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="10">
         <f t="shared" si="0"/>
-        <v>27.309200000000001</v>
-      </c>
-      <c r="E14">
-        <v>27309200</v>
-      </c>
+        <v>40.909550000000003</v>
+      </c>
+      <c r="E14" s="1">
+        <v>43308400</v>
+      </c>
+      <c r="F14" s="1">
+        <v>38510700</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
       <c r="AB14" s="8"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
@@ -3855,13 +4010,24 @@
       <c r="C15" s="7">
         <v>11</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="10">
         <f t="shared" si="0"/>
-        <v>25.7515</v>
-      </c>
-      <c r="E15">
-        <v>25751500</v>
-      </c>
+        <v>36.543550000000003</v>
+      </c>
+      <c r="E15" s="1">
+        <v>40023400</v>
+      </c>
+      <c r="F15" s="1">
+        <v>33063700</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
       <c r="AB15" s="8"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
@@ -3869,13 +4035,24 @@
       <c r="C16" s="7">
         <v>12</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="10">
         <f t="shared" si="0"/>
-        <v>20.646699999999999</v>
-      </c>
-      <c r="E16">
-        <v>20646700</v>
-      </c>
+        <v>36.555199999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <v>37513500</v>
+      </c>
+      <c r="F16" s="1">
+        <v>35596900</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
       <c r="AB16" s="8"/>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.25">
@@ -3883,13 +4060,24 @@
       <c r="C17" s="7">
         <v>13</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="10">
         <f t="shared" si="0"/>
-        <v>23.866299999999999</v>
-      </c>
-      <c r="E17">
-        <v>23866300</v>
-      </c>
+        <v>36.462449999999997</v>
+      </c>
+      <c r="E17" s="1">
+        <v>36667300</v>
+      </c>
+      <c r="F17" s="1">
+        <v>36257600</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
       <c r="AB17" s="8"/>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
@@ -3897,13 +4085,24 @@
       <c r="C18" s="7">
         <v>14</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="10">
         <f t="shared" si="0"/>
-        <v>22.5045</v>
-      </c>
-      <c r="E18">
-        <v>22504500</v>
-      </c>
+        <v>34.431650000000005</v>
+      </c>
+      <c r="E18" s="1">
+        <v>32566000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>36297300</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
       <c r="AB18" s="8"/>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.25">
@@ -3911,13 +4110,24 @@
       <c r="C19" s="7">
         <v>15</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="10">
         <f t="shared" si="0"/>
-        <v>22.041499999999999</v>
-      </c>
-      <c r="E19">
-        <v>22041500</v>
-      </c>
+        <v>33.344149999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>30773800</v>
+      </c>
+      <c r="F19" s="1">
+        <v>35914500</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
       <c r="AB19" s="8"/>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
@@ -3925,13 +4135,24 @@
       <c r="C20" s="7">
         <v>16</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="10">
         <f t="shared" si="0"/>
-        <v>23.369299999999999</v>
-      </c>
-      <c r="E20">
-        <v>23369300</v>
-      </c>
+        <v>32.16545</v>
+      </c>
+      <c r="E20" s="1">
+        <v>31039200</v>
+      </c>
+      <c r="F20" s="1">
+        <v>33291700</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
       <c r="AB20" s="8"/>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
@@ -3939,13 +4160,24 @@
       <c r="C21" s="7">
         <v>17</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="10">
         <f t="shared" si="0"/>
-        <v>22.180900000000001</v>
-      </c>
-      <c r="E21">
-        <v>22180900</v>
-      </c>
+        <v>32.469349999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>30610500</v>
+      </c>
+      <c r="F21" s="1">
+        <v>34328200</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
       <c r="AB21" s="8"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
@@ -3953,13 +4185,24 @@
       <c r="C22" s="7">
         <v>18</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>21.127299999999998</v>
-      </c>
-      <c r="E22">
-        <v>21127300</v>
-      </c>
+        <v>33.022150000000003</v>
+      </c>
+      <c r="E22" s="1">
+        <v>31587900</v>
+      </c>
+      <c r="F22" s="1">
+        <v>34456400</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
       <c r="AB22" s="8"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
@@ -3967,13 +4210,24 @@
       <c r="C23" s="7">
         <v>19</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="10">
         <f t="shared" si="0"/>
-        <v>23.638000000000002</v>
-      </c>
-      <c r="E23">
-        <v>23638000</v>
-      </c>
+        <v>33.774149999999999</v>
+      </c>
+      <c r="E23" s="1">
+        <v>32468900</v>
+      </c>
+      <c r="F23" s="1">
+        <v>35079400</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
       <c r="AB23" s="8"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.25">
@@ -3981,13 +4235,24 @@
       <c r="C24" s="7">
         <v>20</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="10">
         <f t="shared" si="0"/>
-        <v>23.418700000000001</v>
-      </c>
-      <c r="E24">
-        <v>23418700</v>
-      </c>
+        <v>32.425849999999997</v>
+      </c>
+      <c r="E24" s="1">
+        <v>32034500</v>
+      </c>
+      <c r="F24" s="1">
+        <v>32817200</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
       <c r="AB24" s="8"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
@@ -3995,13 +4260,24 @@
       <c r="C25" s="7">
         <v>21</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="10">
         <f t="shared" si="0"/>
-        <v>22.867599999999999</v>
-      </c>
-      <c r="E25">
-        <v>22867600</v>
-      </c>
+        <v>33.772599999999997</v>
+      </c>
+      <c r="E25" s="1">
+        <v>33594600</v>
+      </c>
+      <c r="F25" s="1">
+        <v>33950600</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
       <c r="AB25" s="8"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
@@ -4009,13 +4285,24 @@
       <c r="C26" s="7">
         <v>22</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="10">
         <f t="shared" si="0"/>
-        <v>23.659400000000002</v>
-      </c>
-      <c r="E26">
-        <v>23659400</v>
-      </c>
+        <v>35.000599999999999</v>
+      </c>
+      <c r="E26" s="1">
+        <v>33151000</v>
+      </c>
+      <c r="F26" s="1">
+        <v>36850200</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
       <c r="AB26" s="8"/>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
@@ -4023,13 +4310,24 @@
       <c r="C27" s="7">
         <v>23</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="10">
         <f t="shared" si="0"/>
-        <v>23.844000000000001</v>
-      </c>
-      <c r="E27">
-        <v>23844000</v>
-      </c>
+        <v>34.5334</v>
+      </c>
+      <c r="E27" s="1">
+        <v>31464400</v>
+      </c>
+      <c r="F27" s="1">
+        <v>37602400</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
       <c r="AB27" s="8"/>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
@@ -4037,13 +4335,24 @@
       <c r="C28" s="7">
         <v>24</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="10">
         <f t="shared" si="0"/>
-        <v>22.4389</v>
-      </c>
-      <c r="E28">
-        <v>22438900</v>
-      </c>
+        <v>34.182250000000003</v>
+      </c>
+      <c r="E28" s="1">
+        <v>31338000</v>
+      </c>
+      <c r="F28" s="1">
+        <v>37026500</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
       <c r="AB28" s="8"/>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
@@ -4051,13 +4360,24 @@
       <c r="C29" s="7">
         <v>25</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="10">
         <f t="shared" si="0"/>
-        <v>23.099900000000002</v>
-      </c>
-      <c r="E29">
-        <v>23099900</v>
-      </c>
+        <v>32.964150000000004</v>
+      </c>
+      <c r="E29" s="1">
+        <v>33178300</v>
+      </c>
+      <c r="F29" s="1">
+        <v>32750000</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
       <c r="AB29" s="8"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.25">
@@ -4065,13 +4385,24 @@
       <c r="C30" s="7">
         <v>26</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="10">
         <f t="shared" si="0"/>
-        <v>21.9511</v>
-      </c>
-      <c r="E30">
-        <v>21951100</v>
-      </c>
+        <v>35.02225</v>
+      </c>
+      <c r="E30" s="1">
+        <v>33487600</v>
+      </c>
+      <c r="F30" s="1">
+        <v>36556900</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
       <c r="AB30" s="9"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
@@ -4079,13 +4410,24 @@
       <c r="C31" s="7">
         <v>27</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="10">
         <f t="shared" si="0"/>
-        <v>21.07</v>
-      </c>
-      <c r="E31">
-        <v>21070000</v>
-      </c>
+        <v>33.097749999999998</v>
+      </c>
+      <c r="E31" s="1">
+        <v>30722200</v>
+      </c>
+      <c r="F31" s="1">
+        <v>35473300</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
       <c r="AB31" s="9"/>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
@@ -4093,64 +4435,116 @@
       <c r="C32" s="7">
         <v>28</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="10">
         <f t="shared" si="0"/>
-        <v>23.7775</v>
-      </c>
-      <c r="E32">
-        <v>23777500</v>
-      </c>
+        <v>32.353650000000002</v>
+      </c>
+      <c r="E32" s="1">
+        <v>30693000</v>
+      </c>
+      <c r="F32" s="1">
+        <v>34014300</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
       <c r="AB32" s="9"/>
     </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="7">
         <v>29</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="10">
         <f t="shared" si="0"/>
-        <v>20.517900000000001</v>
-      </c>
-      <c r="E33">
-        <v>20517900</v>
-      </c>
+        <v>33.407849999999996</v>
+      </c>
+      <c r="E33" s="1">
+        <v>32195000</v>
+      </c>
+      <c r="F33" s="1">
+        <v>34620700</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
       <c r="AB33" s="9"/>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="7">
         <v>30</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="10">
         <f t="shared" si="0"/>
-        <v>19.984900000000003</v>
-      </c>
-      <c r="E34">
-        <v>19984900</v>
-      </c>
+        <v>30.833200000000001</v>
+      </c>
+      <c r="E34" s="1">
+        <v>30919500</v>
+      </c>
+      <c r="F34" s="1">
+        <v>30746900</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
       <c r="AB34" s="9"/>
     </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="7">
         <v>31</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="10">
         <f t="shared" si="0"/>
-        <v>21.168400000000002</v>
-      </c>
-      <c r="E35">
-        <v>21168400</v>
-      </c>
+        <v>31.266349999999999</v>
+      </c>
+      <c r="E35" s="1">
+        <v>30731800</v>
+      </c>
+      <c r="F35" s="1">
+        <v>31800900</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
       <c r="AB35" s="9"/>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
       <c r="AB36" s="9"/>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
       <c r="AB37" s="9"/>
     </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>3</v>
       </c>
@@ -4160,32 +4554,71 @@
       <c r="D39" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="5">
-        <f>E40 / 1000 / 1000</f>
-        <v>28.433299999999999</v>
+        <f>SUM(E40:N40) / COUNT(E40:N40)/ 1000 / 1000</f>
+        <v>33.545449999999995</v>
       </c>
       <c r="E40" s="1">
         <v>28433300</v>
       </c>
-    </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F40" s="1">
+        <v>47469700</v>
+      </c>
+      <c r="G40" s="1">
+        <f>AG40/10</f>
+        <v>24733350</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="AG40">
+        <v>247333500</v>
+      </c>
+    </row>
+    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="5">
-        <f>E41 / 1000 / 1000</f>
-        <v>49.979399999999998</v>
+        <f t="shared" ref="D41:D72" si="1">SUM(E41:N41) / COUNT(E41:N41)/ 1000 / 1000</f>
+        <v>102.09437333333332</v>
       </c>
       <c r="E41" s="1">
         <v>49979400</v>
       </c>
-    </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F41" s="1">
+        <v>52847000</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" ref="G41:G72" si="2">AG41/10</f>
+        <v>203456720</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="AG41">
+        <v>2034567200</v>
+      </c>
+    </row>
+    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>5</v>
       </c>
@@ -4193,404 +4626,943 @@
         <v>1</v>
       </c>
       <c r="D42" s="5">
-        <f>E42 / 1000 / 1000</f>
-        <v>32.539000000000001</v>
+        <f t="shared" si="1"/>
+        <v>31.84225</v>
       </c>
       <c r="E42" s="1">
         <v>32539000</v>
       </c>
-    </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F42" s="1">
+        <v>39680700</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="2"/>
+        <v>23307050</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="AG42">
+        <v>233070500</v>
+      </c>
+    </row>
+    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="7">
         <v>2</v>
       </c>
       <c r="D43" s="5">
-        <f>E43 / 1000 / 1000</f>
-        <v>244.04139999999998</v>
+        <f t="shared" si="1"/>
+        <v>286.87023999999997</v>
       </c>
       <c r="E43" s="1">
         <v>244041400</v>
       </c>
-    </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F43" s="1">
+        <v>300531500</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="2"/>
+        <v>316037820</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="AG43">
+        <v>3160378200</v>
+      </c>
+    </row>
+    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="C44" s="7">
         <v>3</v>
       </c>
       <c r="D44" s="5">
-        <f>E44 / 1000 / 1000</f>
-        <v>357.42309999999998</v>
+        <f t="shared" si="1"/>
+        <v>354.46147333333334</v>
       </c>
       <c r="E44" s="1">
         <v>357423100</v>
       </c>
-    </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F44" s="1">
+        <v>331776400</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="2"/>
+        <v>374184920</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="AG44">
+        <v>3741849200</v>
+      </c>
+    </row>
+    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="7">
         <v>4</v>
       </c>
       <c r="D45" s="5">
-        <f>E45 / 1000 / 1000</f>
-        <v>345.21359999999999</v>
+        <f t="shared" si="1"/>
+        <v>377.6347566666667</v>
       </c>
       <c r="E45" s="1">
         <v>345213600</v>
       </c>
-    </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F45" s="1">
+        <v>361984100</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="2"/>
+        <v>425706570</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="AG45">
+        <v>4257065700</v>
+      </c>
+    </row>
+    <row r="46" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="7">
         <v>5</v>
       </c>
       <c r="D46" s="5">
-        <f>E46 / 1000 / 1000</f>
-        <v>409.80440000000004</v>
+        <f t="shared" si="1"/>
+        <v>433.45422333333335</v>
       </c>
       <c r="E46" s="1">
         <v>409804400</v>
       </c>
-    </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F46" s="1">
+        <v>400214900</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="2"/>
+        <v>490343370</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="AG46">
+        <v>4903433700</v>
+      </c>
+    </row>
+    <row r="47" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="C47" s="7">
         <v>6</v>
       </c>
       <c r="D47" s="5">
-        <f>E47 / 1000 / 1000</f>
-        <v>430.00529999999998</v>
+        <f t="shared" si="1"/>
+        <v>437.4499633333333</v>
       </c>
       <c r="E47" s="1">
         <v>430005300</v>
       </c>
-    </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F47" s="1">
+        <v>397526700</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="2"/>
+        <v>484817890</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="AG47">
+        <v>4848178900</v>
+      </c>
+    </row>
+    <row r="48" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" s="7">
         <v>7</v>
       </c>
       <c r="D48" s="5">
-        <f>E48 / 1000 / 1000</f>
-        <v>361.16929999999996</v>
+        <f t="shared" si="1"/>
+        <v>410.13909666666666</v>
       </c>
       <c r="E48" s="1">
         <v>361169300</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="1">
+        <v>396955300</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="2"/>
+        <v>472292690</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="AG48">
+        <v>4722926900</v>
+      </c>
+    </row>
+    <row r="49" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="C49" s="7">
         <v>8</v>
       </c>
       <c r="D49" s="5">
-        <f>E49 / 1000 / 1000</f>
-        <v>356.28479999999996</v>
+        <f t="shared" si="1"/>
+        <v>403.21022999999997</v>
       </c>
       <c r="E49" s="1">
         <v>356284800</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="1">
+        <v>369938800</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="2"/>
+        <v>483407090</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="AG49">
+        <v>4834070900</v>
+      </c>
+    </row>
+    <row r="50" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="7">
         <v>9</v>
       </c>
       <c r="D50" s="5">
-        <f>E50 / 1000 / 1000</f>
-        <v>373.30279999999999</v>
+        <f t="shared" si="1"/>
+        <v>422.72969333333327</v>
       </c>
       <c r="E50" s="1">
         <v>373302800</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="1">
+        <v>394570600</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="2"/>
+        <v>500315680</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="AG50">
+        <v>5003156800</v>
+      </c>
+    </row>
+    <row r="51" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="C51" s="7">
         <v>10</v>
       </c>
       <c r="D51" s="5">
-        <f>E51 / 1000 / 1000</f>
-        <v>366.31540000000001</v>
+        <f t="shared" si="1"/>
+        <v>408.34453999999999</v>
       </c>
       <c r="E51" s="1">
         <v>366315400</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="1">
+        <v>368913500</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="2"/>
+        <v>489804720</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="AG51">
+        <v>4898047200</v>
+      </c>
+    </row>
+    <row r="52" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="C52" s="7">
         <v>11</v>
       </c>
       <c r="D52" s="5">
-        <f>E52 / 1000 / 1000</f>
-        <v>328.73090000000002</v>
+        <f t="shared" si="1"/>
+        <v>382.1543733333333</v>
       </c>
       <c r="E52" s="1">
         <v>328730900</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="1">
+        <v>362363700</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="2"/>
+        <v>455368520</v>
+      </c>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="AG52">
+        <v>4553685200</v>
+      </c>
+    </row>
+    <row r="53" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="C53" s="7">
         <v>12</v>
       </c>
       <c r="D53" s="5">
-        <f>E53 / 1000 / 1000</f>
-        <v>332.58629999999999</v>
+        <f t="shared" si="1"/>
+        <v>373.7577766666667</v>
       </c>
       <c r="E53" s="1">
         <v>332586300</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="1">
+        <v>350982800</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="2"/>
+        <v>437704230</v>
+      </c>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="AG53">
+        <v>4377042300</v>
+      </c>
+    </row>
+    <row r="54" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="C54" s="7">
         <v>13</v>
       </c>
       <c r="D54" s="5">
-        <f>E54 / 1000 / 1000</f>
-        <v>316.14259999999996</v>
+        <f t="shared" si="1"/>
+        <v>349.93829333333332</v>
       </c>
       <c r="E54" s="1">
         <v>316142600</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="1">
+        <v>332955200</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="2"/>
+        <v>400717080</v>
+      </c>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="AG54">
+        <v>4007170800</v>
+      </c>
+    </row>
+    <row r="55" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="7">
         <v>14</v>
       </c>
       <c r="D55" s="5">
-        <f>E55 / 1000 / 1000</f>
-        <v>329.6748</v>
+        <f t="shared" si="1"/>
+        <v>349.15191666666669</v>
       </c>
       <c r="E55" s="1">
         <v>329674800</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="1">
+        <v>330660700</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="2"/>
+        <v>387120250</v>
+      </c>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="AG55">
+        <v>3871202500</v>
+      </c>
+    </row>
+    <row r="56" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="7">
         <v>15</v>
       </c>
       <c r="D56" s="5">
-        <f>E56 / 1000 / 1000</f>
-        <v>311.63069999999999</v>
+        <f t="shared" si="1"/>
+        <v>334.30834999999996</v>
       </c>
       <c r="E56" s="1">
         <v>311630700</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="1">
+        <v>319788100</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="2"/>
+        <v>371506250</v>
+      </c>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="AG56">
+        <v>3715062500</v>
+      </c>
+    </row>
+    <row r="57" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="C57" s="7">
         <v>16</v>
       </c>
       <c r="D57" s="5">
-        <f>E57 / 1000 / 1000</f>
-        <v>304.33800000000002</v>
+        <f t="shared" si="1"/>
+        <v>320.80375666666669</v>
       </c>
       <c r="E57" s="1">
         <v>304338000</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="1">
+        <v>305499100</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="2"/>
+        <v>352574170</v>
+      </c>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="AG57">
+        <v>3525741700</v>
+      </c>
+    </row>
+    <row r="58" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="C58" s="7">
         <v>17</v>
       </c>
       <c r="D58" s="5">
-        <f>E58 / 1000 / 1000</f>
-        <v>316.92399999999998</v>
+        <f t="shared" si="1"/>
+        <v>330.76777000000004</v>
       </c>
       <c r="E58" s="1">
         <v>316924000</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="1">
+        <v>310097300</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="2"/>
+        <v>365282010</v>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="AG58">
+        <v>3652820100</v>
+      </c>
+    </row>
+    <row r="59" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="C59" s="7">
         <v>18</v>
       </c>
       <c r="D59" s="5">
-        <f>E59 / 1000 / 1000</f>
-        <v>300.46609999999998</v>
+        <f t="shared" si="1"/>
+        <v>329.44851</v>
       </c>
       <c r="E59" s="1">
         <v>300466100</v>
       </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="1">
+        <v>312368400</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="2"/>
+        <v>375511030</v>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="AG59">
+        <v>3755110300</v>
+      </c>
+    </row>
+    <row r="60" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="C60" s="7">
         <v>19</v>
       </c>
       <c r="D60" s="5">
-        <f>E60 / 1000 / 1000</f>
-        <v>303.16070000000002</v>
+        <f t="shared" si="1"/>
+        <v>318.64961999999997</v>
       </c>
       <c r="E60" s="1">
         <v>303160700</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="1">
+        <v>301508200</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="2"/>
+        <v>351279960</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="AG60">
+        <v>3512799600</v>
+      </c>
+    </row>
+    <row r="61" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="C61" s="7">
         <v>20</v>
       </c>
       <c r="D61" s="5">
-        <f>E61 / 1000 / 1000</f>
-        <v>297.2799</v>
+        <f t="shared" si="1"/>
+        <v>316.99907000000002</v>
       </c>
       <c r="E61" s="1">
         <v>297279900</v>
       </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="1">
+        <v>296456600</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="2"/>
+        <v>357260710</v>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="AG61">
+        <v>3572607100</v>
+      </c>
+    </row>
+    <row r="62" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="C62" s="7">
         <v>21</v>
       </c>
       <c r="D62" s="5">
-        <f>E62 / 1000 / 1000</f>
-        <v>304.0249</v>
+        <f t="shared" si="1"/>
+        <v>313.93516999999997</v>
       </c>
       <c r="E62" s="1">
         <v>304024900</v>
       </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="1">
+        <v>297238300</v>
+      </c>
+      <c r="G62" s="1">
+        <f t="shared" si="2"/>
+        <v>340542310</v>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="AG62">
+        <v>3405423100</v>
+      </c>
+    </row>
+    <row r="63" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="C63" s="7">
         <v>22</v>
       </c>
       <c r="D63" s="5">
-        <f>E63 / 1000 / 1000</f>
-        <v>302.67720000000003</v>
+        <f t="shared" si="1"/>
+        <v>326.15464666666668</v>
       </c>
       <c r="E63" s="1">
         <v>302677200</v>
       </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="1">
+        <v>312758700</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="2"/>
+        <v>363028040</v>
+      </c>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="AG63">
+        <v>3630280400</v>
+      </c>
+    </row>
+    <row r="64" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="C64" s="7">
         <v>23</v>
       </c>
       <c r="D64" s="5">
-        <f>E64 / 1000 / 1000</f>
-        <v>297.9658</v>
+        <f t="shared" si="1"/>
+        <v>317.04913666666664</v>
       </c>
       <c r="E64" s="1">
         <v>297965800</v>
       </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="1">
+        <v>303472000</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="2"/>
+        <v>349709610</v>
+      </c>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="AG64">
+        <v>3497096100</v>
+      </c>
+    </row>
+    <row r="65" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="C65" s="7">
         <v>24</v>
       </c>
       <c r="D65" s="5">
-        <f>E65 / 1000 / 1000</f>
-        <v>309.1771</v>
+        <f t="shared" si="1"/>
+        <v>322.84330666666671</v>
       </c>
       <c r="E65" s="1">
         <v>309177100</v>
       </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="1">
+        <v>313048000</v>
+      </c>
+      <c r="G65" s="1">
+        <f t="shared" si="2"/>
+        <v>346304820</v>
+      </c>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="AG65">
+        <v>3463048200</v>
+      </c>
+    </row>
+    <row r="66" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="C66" s="7">
         <v>25</v>
       </c>
       <c r="D66" s="5">
-        <f>E66 / 1000 / 1000</f>
-        <v>303.77499999999998</v>
+        <f t="shared" si="1"/>
+        <v>362.56063666666665</v>
       </c>
       <c r="E66" s="1">
         <v>303775000</v>
       </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="1">
+        <v>431818300</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" si="2"/>
+        <v>352088610</v>
+      </c>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="AG66">
+        <v>3520886100</v>
+      </c>
+    </row>
+    <row r="67" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="C67" s="7">
         <v>26</v>
       </c>
       <c r="D67" s="5">
-        <f>E67 / 1000 / 1000</f>
-        <v>313.49650000000003</v>
+        <f t="shared" si="1"/>
+        <v>327.00149333333331</v>
       </c>
       <c r="E67" s="1">
         <v>313496500</v>
       </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="1">
+        <v>322596400</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" si="2"/>
+        <v>344911580</v>
+      </c>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="AG67">
+        <v>3449115800</v>
+      </c>
+    </row>
+    <row r="68" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="C68" s="7">
         <v>27</v>
       </c>
       <c r="D68" s="5">
-        <f>E68 / 1000 / 1000</f>
-        <v>299.80829999999997</v>
+        <f t="shared" si="1"/>
+        <v>318.19207333333333</v>
       </c>
       <c r="E68" s="1">
         <v>299808300</v>
       </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="1">
+        <v>306056000</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" si="2"/>
+        <v>348711920</v>
+      </c>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="AG68">
+        <v>3487119200</v>
+      </c>
+    </row>
+    <row r="69" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="C69" s="7">
         <v>28</v>
       </c>
       <c r="D69" s="5">
-        <f>E69 / 1000 / 1000</f>
-        <v>313.28709999999995</v>
+        <f t="shared" si="1"/>
+        <v>328.18165000000005</v>
       </c>
       <c r="E69" s="1">
         <v>313287100</v>
       </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="1">
+        <v>326549700</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" si="2"/>
+        <v>344708150</v>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="AG69">
+        <v>3447081500</v>
+      </c>
+    </row>
+    <row r="70" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="C70" s="7">
         <v>29</v>
       </c>
       <c r="D70" s="5">
-        <f>E70 / 1000 / 1000</f>
-        <v>304.2038</v>
+        <f t="shared" si="1"/>
+        <v>360.72090999999995</v>
       </c>
       <c r="E70" s="1">
         <v>304203800</v>
       </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="1">
+        <v>426975400</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" si="2"/>
+        <v>350983530</v>
+      </c>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="AG70">
+        <v>3509835300</v>
+      </c>
+    </row>
+    <row r="71" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="C71" s="7">
         <v>30</v>
       </c>
       <c r="D71" s="5">
-        <f>E71 / 1000 / 1000</f>
-        <v>306.58709999999996</v>
+        <f t="shared" si="1"/>
+        <v>360.95258000000001</v>
       </c>
       <c r="E71" s="1">
         <v>306587100</v>
       </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="1">
+        <v>417802500</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="2"/>
+        <v>358468140</v>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="AG71">
+        <v>3584681400</v>
+      </c>
+    </row>
+    <row r="72" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="C72" s="7">
         <v>31</v>
       </c>
       <c r="D72" s="5">
-        <f>E72 / 1000 / 1000</f>
-        <v>304.6198</v>
+        <f t="shared" si="1"/>
+        <v>342.80452000000002</v>
       </c>
       <c r="E72" s="1">
         <v>304619800</v>
       </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="1">
+        <v>364964000</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="2"/>
+        <v>358829760</v>
+      </c>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="AG72">
+        <v>3588297600</v>
+      </c>
+    </row>
+    <row r="73" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>6</v>
       </c>
@@ -4600,32 +5572,64 @@
       <c r="D76" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>0</v>
       </c>
       <c r="D77" s="5">
-        <f t="shared" ref="D77:D109" si="1">E77 / 1000 / 1000</f>
-        <v>212.6105</v>
-      </c>
-      <c r="E77">
+        <f>SUM(E77:N77) / COUNT(E77:N77)/ 1000 / 1000</f>
+        <v>213.75745000000001</v>
+      </c>
+      <c r="E77" s="1">
         <v>212610500</v>
       </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="1">
+        <v>200194100</v>
+      </c>
+      <c r="G77" s="1">
+        <v>247898100</v>
+      </c>
+      <c r="H77" s="1">
+        <v>194327100</v>
+      </c>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+    </row>
+    <row r="78" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>2</v>
       </c>
       <c r="D78" s="5">
-        <f t="shared" si="1"/>
-        <v>269.43540000000002</v>
-      </c>
-      <c r="E78">
+        <f t="shared" ref="D78:D109" si="3">SUM(E78:N78) / COUNT(E78:N78)/ 1000 / 1000</f>
+        <v>968.4126</v>
+      </c>
+      <c r="E78" s="1">
         <v>269435400</v>
       </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F78" s="1">
+        <v>270762400</v>
+      </c>
+      <c r="G78" s="1">
+        <v>302943500</v>
+      </c>
+      <c r="H78" s="12">
+        <v>3030509100</v>
+      </c>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+    </row>
+    <row r="79" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="s">
         <v>5</v>
       </c>
@@ -4633,402 +5637,960 @@
         <v>1</v>
       </c>
       <c r="D79" s="5">
-        <f t="shared" si="1"/>
-        <v>235.7038</v>
-      </c>
-      <c r="E79">
+        <f t="shared" si="3"/>
+        <v>220.41729999999998</v>
+      </c>
+      <c r="E79" s="1">
         <v>235703800</v>
       </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F79" s="1">
+        <v>203598400</v>
+      </c>
+      <c r="G79" s="1">
+        <v>235587900</v>
+      </c>
+      <c r="H79" s="1">
+        <v>206779100</v>
+      </c>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+    </row>
+    <row r="80" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="C80" s="7">
         <v>2</v>
       </c>
       <c r="D80" s="5">
-        <f t="shared" si="1"/>
-        <v>2504.6324</v>
-      </c>
-      <c r="E80">
+        <f t="shared" si="3"/>
+        <v>2520.1049750000002</v>
+      </c>
+      <c r="E80" s="1">
         <v>2504632400</v>
       </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F80" s="1">
+        <v>2450270000</v>
+      </c>
+      <c r="G80" s="1">
+        <v>2526063600</v>
+      </c>
+      <c r="H80" s="1">
+        <v>2599453900</v>
+      </c>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="C81" s="7">
         <v>3</v>
       </c>
       <c r="D81" s="5">
-        <f t="shared" si="1"/>
-        <v>3336.4681</v>
-      </c>
-      <c r="E81">
+        <f t="shared" si="3"/>
+        <v>3125.7725</v>
+      </c>
+      <c r="E81" s="1">
         <v>3336468100</v>
       </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F81" s="1">
+        <v>3084322800</v>
+      </c>
+      <c r="G81" s="1">
+        <v>3100493200</v>
+      </c>
+      <c r="H81" s="1">
+        <v>2981805900</v>
+      </c>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="C82" s="7">
         <v>4</v>
       </c>
       <c r="D82" s="5">
-        <f t="shared" si="1"/>
-        <v>4147.0815000000002</v>
-      </c>
-      <c r="E82">
+        <f t="shared" si="3"/>
+        <v>3732.9300750000002</v>
+      </c>
+      <c r="E82" s="1">
         <v>4147081500</v>
       </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F82" s="1">
+        <v>3557056000</v>
+      </c>
+      <c r="G82" s="1">
+        <v>3796597100</v>
+      </c>
+      <c r="H82" s="1">
+        <v>3430985700</v>
+      </c>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="C83" s="7">
         <v>5</v>
       </c>
       <c r="D83" s="5">
-        <f t="shared" si="1"/>
-        <v>4164.6562000000004</v>
-      </c>
-      <c r="E83">
+        <f t="shared" si="3"/>
+        <v>3659.3316500000001</v>
+      </c>
+      <c r="E83" s="1">
         <v>4164656200</v>
       </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F83" s="1">
+        <v>3832573500</v>
+      </c>
+      <c r="G83" s="1">
+        <v>2745475200</v>
+      </c>
+      <c r="H83" s="1">
+        <v>3894621700</v>
+      </c>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="C84" s="7">
         <v>6</v>
       </c>
       <c r="D84" s="5">
-        <f t="shared" si="1"/>
-        <v>4052.0135</v>
-      </c>
-      <c r="E84">
+        <f t="shared" si="3"/>
+        <v>3422.7775499999998</v>
+      </c>
+      <c r="E84" s="1">
         <v>4052013500</v>
       </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F84" s="1">
+        <v>4009272900</v>
+      </c>
+      <c r="G84" s="1">
+        <v>1843191600</v>
+      </c>
+      <c r="H84" s="1">
+        <v>3786632200</v>
+      </c>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="C85" s="7">
         <v>7</v>
       </c>
       <c r="D85" s="5">
-        <f t="shared" si="1"/>
-        <v>3544.3163999999997</v>
-      </c>
-      <c r="E85">
+        <f t="shared" si="3"/>
+        <v>3099.3313750000002</v>
+      </c>
+      <c r="E85" s="1">
         <v>3544316400</v>
       </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F85" s="1">
+        <v>3644485400</v>
+      </c>
+      <c r="G85" s="1">
+        <v>1724433200</v>
+      </c>
+      <c r="H85" s="1">
+        <v>3484090500</v>
+      </c>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="C86" s="7">
         <v>8</v>
       </c>
       <c r="D86" s="5">
-        <f t="shared" si="1"/>
-        <v>3630.1227999999996</v>
-      </c>
-      <c r="E86">
+        <f t="shared" si="3"/>
+        <v>3121.9437749999997</v>
+      </c>
+      <c r="E86" s="1">
         <v>3630122800</v>
       </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F86" s="1">
+        <v>3601258600</v>
+      </c>
+      <c r="G86" s="1">
+        <v>1658865100</v>
+      </c>
+      <c r="H86" s="1">
+        <v>3597528600</v>
+      </c>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+    </row>
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="C87" s="7">
         <v>9</v>
       </c>
       <c r="D87" s="5">
-        <f t="shared" si="1"/>
-        <v>3661.4503999999997</v>
-      </c>
-      <c r="E87">
+        <f t="shared" si="3"/>
+        <v>3171.8808749999998</v>
+      </c>
+      <c r="E87" s="1">
         <v>3661450400</v>
       </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="1">
+        <v>3747830500</v>
+      </c>
+      <c r="G87" s="1">
+        <v>1665935700</v>
+      </c>
+      <c r="H87" s="1">
+        <v>3612306900</v>
+      </c>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="C88" s="7">
         <v>10</v>
       </c>
       <c r="D88" s="5">
-        <f t="shared" si="1"/>
-        <v>3592.1977000000002</v>
-      </c>
-      <c r="E88">
+        <f t="shared" si="3"/>
+        <v>3155.7731749999998</v>
+      </c>
+      <c r="E88" s="1">
         <v>3592197700</v>
       </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F88" s="1">
+        <v>3690174500</v>
+      </c>
+      <c r="G88" s="1">
+        <v>1657554100</v>
+      </c>
+      <c r="H88" s="1">
+        <v>3683166400</v>
+      </c>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="C89" s="7">
         <v>11</v>
       </c>
       <c r="D89" s="5">
-        <f t="shared" si="1"/>
-        <v>3378.9196000000002</v>
-      </c>
-      <c r="E89">
+        <f t="shared" si="3"/>
+        <v>3163.0625249999998</v>
+      </c>
+      <c r="E89" s="1">
         <v>3378919600</v>
       </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F89" s="1">
+        <v>3613767200</v>
+      </c>
+      <c r="G89" s="1">
+        <v>2208779600</v>
+      </c>
+      <c r="H89" s="1">
+        <v>3450783700</v>
+      </c>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
       <c r="C90" s="7">
         <v>12</v>
       </c>
       <c r="D90" s="5">
-        <f t="shared" si="1"/>
-        <v>3440.2542000000003</v>
-      </c>
-      <c r="E90">
+        <f t="shared" si="3"/>
+        <v>3258.3580499999998</v>
+      </c>
+      <c r="E90" s="1">
         <v>3440254200</v>
       </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F90" s="1">
+        <v>2896792500</v>
+      </c>
+      <c r="G90" s="1">
+        <v>3298661700</v>
+      </c>
+      <c r="H90" s="1">
+        <v>3397723800</v>
+      </c>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+    </row>
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
       <c r="C91" s="7">
         <v>13</v>
       </c>
       <c r="D91" s="5">
-        <f t="shared" si="1"/>
-        <v>4122.3252999999995</v>
-      </c>
-      <c r="E91">
+        <f t="shared" si="3"/>
+        <v>3264.6103499999999</v>
+      </c>
+      <c r="E91" s="1">
         <v>4122325300</v>
       </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F91" s="1">
+        <v>2623193700</v>
+      </c>
+      <c r="G91" s="1">
+        <v>3075066300</v>
+      </c>
+      <c r="H91" s="1">
+        <v>3237856100</v>
+      </c>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+    </row>
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
       <c r="C92" s="7">
         <v>14</v>
       </c>
       <c r="D92" s="5">
-        <f t="shared" si="1"/>
-        <v>4121.1535999999996</v>
-      </c>
-      <c r="E92">
+        <f t="shared" si="3"/>
+        <v>3187.1091499999998</v>
+      </c>
+      <c r="E92" s="1">
         <v>4121153600</v>
       </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F92" s="1">
+        <v>2596220000</v>
+      </c>
+      <c r="G92" s="1">
+        <v>2850270300</v>
+      </c>
+      <c r="H92" s="1">
+        <v>3180792700</v>
+      </c>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+    </row>
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
       <c r="C93" s="7">
         <v>15</v>
       </c>
       <c r="D93" s="5">
-        <f t="shared" si="1"/>
-        <v>4722.8922000000002</v>
-      </c>
-      <c r="E93">
+        <f t="shared" si="3"/>
+        <v>3352.389525</v>
+      </c>
+      <c r="E93" s="1">
         <v>4722892200</v>
       </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F93" s="1">
+        <v>2602370400</v>
+      </c>
+      <c r="G93" s="1">
+        <v>3033491500</v>
+      </c>
+      <c r="H93" s="1">
+        <v>3050804000</v>
+      </c>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+    </row>
+    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
       <c r="C94" s="7">
         <v>16</v>
       </c>
       <c r="D94" s="5">
-        <f t="shared" si="1"/>
-        <v>4327.9656999999997</v>
-      </c>
-      <c r="E94">
+        <f t="shared" si="3"/>
+        <v>3198.14455</v>
+      </c>
+      <c r="E94" s="1">
         <v>4327965700</v>
       </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F94" s="1">
+        <v>2550048200</v>
+      </c>
+      <c r="G94" s="1">
+        <v>2966792700</v>
+      </c>
+      <c r="H94" s="1">
+        <v>2947771600</v>
+      </c>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+    </row>
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
       <c r="C95" s="7">
         <v>17</v>
       </c>
       <c r="D95" s="5">
-        <f t="shared" si="1"/>
-        <v>4230.5754999999999</v>
-      </c>
-      <c r="E95">
+        <f t="shared" si="3"/>
+        <v>3168.8187749999997</v>
+      </c>
+      <c r="E95" s="1">
         <v>4230575500</v>
       </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F95" s="1">
+        <v>2585103000</v>
+      </c>
+      <c r="G95" s="1">
+        <v>2896770700</v>
+      </c>
+      <c r="H95" s="1">
+        <v>2962825900</v>
+      </c>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+    </row>
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B96" s="6"/>
       <c r="C96" s="7">
         <v>18</v>
       </c>
       <c r="D96" s="5">
-        <f t="shared" si="1"/>
-        <v>4175.8537000000006</v>
-      </c>
-      <c r="E96">
+        <f t="shared" si="3"/>
+        <v>3163.9285249999998</v>
+      </c>
+      <c r="E96" s="1">
         <v>4175853700</v>
       </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F96" s="1">
+        <v>2535646900</v>
+      </c>
+      <c r="G96" s="1">
+        <v>2962296700</v>
+      </c>
+      <c r="H96" s="1">
+        <v>2981916800</v>
+      </c>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+    </row>
+    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
       <c r="C97" s="7">
         <v>19</v>
       </c>
       <c r="D97" s="5">
-        <f t="shared" si="1"/>
-        <v>4119.384</v>
-      </c>
-      <c r="E97">
+        <f t="shared" si="3"/>
+        <v>3142.725375</v>
+      </c>
+      <c r="E97" s="1">
         <v>4119384000</v>
       </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F97" s="1">
+        <v>2549100300</v>
+      </c>
+      <c r="G97" s="1">
+        <v>2924636300</v>
+      </c>
+      <c r="H97" s="1">
+        <v>2977780900</v>
+      </c>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+    </row>
+    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
       <c r="C98" s="7">
         <v>20</v>
       </c>
       <c r="D98" s="5">
-        <f t="shared" si="1"/>
-        <v>4490.6172999999999</v>
-      </c>
-      <c r="E98">
+        <f t="shared" si="3"/>
+        <v>3241.3328999999999</v>
+      </c>
+      <c r="E98" s="1">
         <v>4490617300</v>
       </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F98" s="1">
+        <v>2602292400</v>
+      </c>
+      <c r="G98" s="1">
+        <v>2881233200</v>
+      </c>
+      <c r="H98" s="1">
+        <v>2991188700</v>
+      </c>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+    </row>
+    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
       <c r="C99" s="7">
         <v>21</v>
       </c>
       <c r="D99" s="5">
-        <f t="shared" si="1"/>
-        <v>4326.2375999999995</v>
-      </c>
-      <c r="E99">
+        <f t="shared" si="3"/>
+        <v>3198.67355</v>
+      </c>
+      <c r="E99" s="1">
         <v>4326237600</v>
       </c>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F99" s="1">
+        <v>2567678400</v>
+      </c>
+      <c r="G99" s="1">
+        <v>2945734800</v>
+      </c>
+      <c r="H99" s="1">
+        <v>2955043400</v>
+      </c>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+    </row>
+    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
       <c r="C100" s="7">
         <v>22</v>
       </c>
       <c r="D100" s="5">
-        <f t="shared" si="1"/>
-        <v>4635.0565999999999</v>
-      </c>
-      <c r="E100">
+        <f t="shared" si="3"/>
+        <v>3290.8587000000002</v>
+      </c>
+      <c r="E100" s="1">
         <v>4635056600</v>
       </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F100" s="1">
+        <v>2615001800</v>
+      </c>
+      <c r="G100" s="1">
+        <v>2896144000</v>
+      </c>
+      <c r="H100" s="1">
+        <v>3017232400</v>
+      </c>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+    </row>
+    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
       <c r="C101" s="7">
         <v>23</v>
       </c>
       <c r="D101" s="5">
-        <f t="shared" si="1"/>
-        <v>4084.4297999999999</v>
-      </c>
-      <c r="E101">
+        <f t="shared" si="3"/>
+        <v>3143.5763999999999</v>
+      </c>
+      <c r="E101" s="1">
         <v>4084429800</v>
       </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F101" s="1">
+        <v>2637310900</v>
+      </c>
+      <c r="G101" s="1">
+        <v>2872639200</v>
+      </c>
+      <c r="H101" s="1">
+        <v>2979925700</v>
+      </c>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+    </row>
+    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B102" s="6"/>
       <c r="C102" s="7">
         <v>24</v>
       </c>
       <c r="D102" s="5">
-        <f t="shared" si="1"/>
-        <v>2444.9911000000002</v>
-      </c>
-      <c r="E102">
+        <f t="shared" si="3"/>
+        <v>2768.4515499999998</v>
+      </c>
+      <c r="E102" s="1">
         <v>2444991100</v>
       </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F102" s="1">
+        <v>2641374300</v>
+      </c>
+      <c r="G102" s="1">
+        <v>3042137000</v>
+      </c>
+      <c r="H102" s="1">
+        <v>2945303800</v>
+      </c>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+    </row>
+    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B103" s="6"/>
       <c r="C103" s="7">
         <v>25</v>
       </c>
       <c r="D103" s="5">
-        <f t="shared" si="1"/>
-        <v>1654.5496000000001</v>
-      </c>
-      <c r="E103">
+        <f t="shared" si="3"/>
+        <v>2509.0195750000003</v>
+      </c>
+      <c r="E103" s="1">
         <v>1654549600</v>
       </c>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F103" s="1">
+        <v>2570247100</v>
+      </c>
+      <c r="G103" s="1">
+        <v>2887181700</v>
+      </c>
+      <c r="H103" s="1">
+        <v>2924099900</v>
+      </c>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+    </row>
+    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
       <c r="C104" s="7">
         <v>26</v>
       </c>
       <c r="D104" s="5">
-        <f t="shared" si="1"/>
-        <v>1788.7021000000002</v>
-      </c>
-      <c r="E104">
+        <f t="shared" si="3"/>
+        <v>2572.3301749999996</v>
+      </c>
+      <c r="E104" s="1">
         <v>1788702100</v>
       </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F104" s="1">
+        <v>2677916900</v>
+      </c>
+      <c r="G104" s="1">
+        <v>2923334300</v>
+      </c>
+      <c r="H104" s="1">
+        <v>2899367400</v>
+      </c>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+    </row>
+    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B105" s="6"/>
       <c r="C105" s="7">
         <v>27</v>
       </c>
       <c r="D105" s="5">
-        <f t="shared" si="1"/>
-        <v>2013.2529</v>
-      </c>
-      <c r="E105">
+        <f t="shared" si="3"/>
+        <v>2580.5604500000004</v>
+      </c>
+      <c r="E105" s="1">
         <v>2013252900</v>
       </c>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F105" s="1">
+        <v>2571752300</v>
+      </c>
+      <c r="G105" s="1">
+        <v>2863135900</v>
+      </c>
+      <c r="H105" s="1">
+        <v>2874100700</v>
+      </c>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+    </row>
+    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B106" s="6"/>
       <c r="C106" s="7">
         <v>28</v>
       </c>
       <c r="D106" s="5">
-        <f t="shared" si="1"/>
-        <v>2199.1061</v>
-      </c>
-      <c r="E106">
+        <f t="shared" si="3"/>
+        <v>2763.2431499999998</v>
+      </c>
+      <c r="E106" s="1">
         <v>2199106100</v>
       </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F106" s="1">
+        <v>3019589100</v>
+      </c>
+      <c r="G106" s="1">
+        <v>2925924600</v>
+      </c>
+      <c r="H106" s="1">
+        <v>2908352800</v>
+      </c>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+    </row>
+    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B107" s="6"/>
       <c r="C107" s="7">
         <v>29</v>
       </c>
       <c r="D107" s="5">
-        <f t="shared" si="1"/>
-        <v>3448.3698999999997</v>
-      </c>
-      <c r="E107">
+        <f t="shared" si="3"/>
+        <v>3042.1008500000003</v>
+      </c>
+      <c r="E107" s="1">
         <v>3448369900</v>
       </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F107" s="1">
+        <v>2900651000</v>
+      </c>
+      <c r="G107" s="1">
+        <v>2856299300</v>
+      </c>
+      <c r="H107" s="1">
+        <v>2963083200</v>
+      </c>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+    </row>
+    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B108" s="6"/>
       <c r="C108" s="7">
         <v>30</v>
       </c>
       <c r="D108" s="5">
-        <f t="shared" si="1"/>
-        <v>4435.7227000000003</v>
-      </c>
-      <c r="E108">
+        <f t="shared" si="3"/>
+        <v>3287.0614500000001</v>
+      </c>
+      <c r="E108" s="1">
         <v>4435722700</v>
       </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F108" s="1">
+        <v>2899609100</v>
+      </c>
+      <c r="G108" s="1">
+        <v>2922044800</v>
+      </c>
+      <c r="H108" s="1">
+        <v>2890869200</v>
+      </c>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B109" s="6"/>
       <c r="C109" s="7">
         <v>31</v>
       </c>
       <c r="D109" s="5">
-        <f t="shared" si="1"/>
-        <v>4172.9618</v>
-      </c>
-      <c r="E109">
+        <f t="shared" si="3"/>
+        <v>3291.7092000000002</v>
+      </c>
+      <c r="E109" s="1">
         <v>4172961800</v>
       </c>
+      <c r="F109" s="1">
+        <v>3183231400</v>
+      </c>
+      <c r="G109" s="1">
+        <v>2893935200</v>
+      </c>
+      <c r="H109" s="1">
+        <v>2916708400</v>
+      </c>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="8"/>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="8"/>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="8"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="8"/>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="8"/>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="8"/>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="8"/>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="8"/>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E125" s="8"/>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E126" s="8"/>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="8"/>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E128" s="8"/>
+    </row>
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E129" s="8"/>
+    </row>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E130" s="8"/>
+    </row>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E131" s="8"/>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="8"/>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E133" s="8"/>
+    </row>
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E134" s="8"/>
+    </row>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E135" s="8"/>
+    </row>
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E136" s="8"/>
+    </row>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E137" s="8"/>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E138" s="8"/>
+    </row>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E139" s="8"/>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E140" s="9"/>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E141" s="9"/>
+    </row>
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E142" s="9"/>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E143" s="9"/>
+    </row>
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E144" s="9"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E145" s="9"/>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E146" s="9"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E147" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
return Atomic Boolean and set good array in test.
</commit_message>
<xml_diff>
--- a/Task_2_1_1/time.xlsx
+++ b/Task_2_1_1/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\NSU\OOP\Task_2_1_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE64AC8F-EB5A-4CE8-B07F-BD227DAD8706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C783D4B4-3095-466D-98A8-86322C31BB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D5ABC52E-7C61-45CD-9E16-B81EF21C7B9D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>Usual</t>
   </si>
@@ -57,7 +57,7 @@
     <t>arr.length = 1kk</t>
   </si>
   <si>
-    <t>с 10-кратным повторением (поделил на 10 потом)</t>
+    <t>arr.length = 100k</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +87,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -144,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -158,6 +167,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -274,216 +284,205 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Лист1!$C$40:$C$72</c:f>
-              <c:strCache>
-                <c:ptCount val="33"/>
+            <c:numRef>
+              <c:f>Лист1!$C$42:$C$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>Usual</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Optimus (Stream)</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>26</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="32">
                   <c:v>31</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$40:$D$72</c:f>
+              <c:f>Лист1!$D$42:$D$72</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>33.545449999999995</c:v>
+                  <c:v>0.36516666666666669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102.09437333333332</c:v>
+                  <c:v>0.33176666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.84225</c:v>
+                  <c:v>0.4088</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>286.87023999999997</c:v>
+                  <c:v>0.4234</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>354.46147333333334</c:v>
+                  <c:v>0.4264</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>377.6347566666667</c:v>
+                  <c:v>0.435</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>433.45422333333335</c:v>
+                  <c:v>0.43969999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>437.4499633333333</c:v>
+                  <c:v>0.55210000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>410.13909666666666</c:v>
+                  <c:v>0.56720000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>403.21022999999997</c:v>
+                  <c:v>0.60363333333333336</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>422.72969333333327</c:v>
+                  <c:v>0.64136666666666664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>408.34453999999999</c:v>
+                  <c:v>0.69653333333333345</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>382.1543733333333</c:v>
+                  <c:v>0.73799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>373.7577766666667</c:v>
+                  <c:v>1.2566666666666668</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>349.93829333333332</c:v>
+                  <c:v>0.82023333333333337</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>349.15191666666669</c:v>
+                  <c:v>0.84033333333333338</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>334.30834999999996</c:v>
+                  <c:v>0.95563333333333333</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>320.80375666666669</c:v>
+                  <c:v>1.7404999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>330.76777000000004</c:v>
+                  <c:v>2.1255666666666668</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>329.44851</c:v>
+                  <c:v>1.2076333333333331</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>318.64961999999997</c:v>
+                  <c:v>2.4201333333333337</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>316.99907000000002</c:v>
+                  <c:v>1.5143333333333333</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>313.93516999999997</c:v>
+                  <c:v>1.5115666666666667</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>326.15464666666668</c:v>
+                  <c:v>1.2510999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>317.04913666666664</c:v>
+                  <c:v>1.3248333333333333</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>322.84330666666671</c:v>
+                  <c:v>1.5193666666666668</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>362.56063666666665</c:v>
+                  <c:v>1.7243666666666668</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>327.00149333333331</c:v>
+                  <c:v>1.4458666666666669</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>318.19207333333333</c:v>
+                  <c:v>1.4727666666666666</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>328.18165000000005</c:v>
+                  <c:v>1.4951333333333332</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>360.72090999999995</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>360.95258000000001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>342.80452000000002</c:v>
+                  <c:v>1.6969333333333332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1355,103 +1354,103 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>23.286999999999999</c:v>
+                  <c:v>4033.3507999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.515500000000003</c:v>
+                  <c:v>2361.6039999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.363849999999999</c:v>
+                  <c:v>4093.4922999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.317999999999998</c:v>
+                  <c:v>2023.3779</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.698250000000002</c:v>
+                  <c:v>4467.8284000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.61795</c:v>
+                  <c:v>4519.5195999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.782249999999998</c:v>
+                  <c:v>4636.1889000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.986050000000006</c:v>
+                  <c:v>4794.2619000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42.423250000000003</c:v>
+                  <c:v>5055.3064999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43.198250000000002</c:v>
+                  <c:v>5118.8723</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37.142400000000002</c:v>
+                  <c:v>5304.3768</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.909550000000003</c:v>
+                  <c:v>5386.2038000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.543550000000003</c:v>
+                  <c:v>5461.3427000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.555199999999999</c:v>
+                  <c:v>5596.9142000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.462449999999997</c:v>
+                  <c:v>5718.4560000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.431650000000005</c:v>
+                  <c:v>5848.3908000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33.344149999999999</c:v>
+                  <c:v>5888.8244999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.16545</c:v>
+                  <c:v>5869.1355999999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.469349999999999</c:v>
+                  <c:v>5891.8882000000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33.022150000000003</c:v>
+                  <c:v>5939.5755999999992</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>33.774149999999999</c:v>
+                  <c:v>5869.9935999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>32.425849999999997</c:v>
+                  <c:v>6478.9552999999996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>33.772599999999997</c:v>
+                  <c:v>6675.9492</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35.000599999999999</c:v>
+                  <c:v>6655.8872999999994</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34.5334</c:v>
+                  <c:v>6223.5045</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>34.182250000000003</c:v>
+                  <c:v>5958.7987999999996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>32.964150000000004</c:v>
+                  <c:v>5958.3064999999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>35.02225</c:v>
+                  <c:v>5965.9070999999994</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>33.097749999999998</c:v>
+                  <c:v>5958.8387000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>32.353650000000002</c:v>
+                  <c:v>5962.8292999999994</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>33.407849999999996</c:v>
+                  <c:v>5986.7290000000003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>30.833200000000001</c:v>
+                  <c:v>5987.3458000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>31.266349999999999</c:v>
+                  <c:v>5979.7764999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1634,6 +1633,773 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>в</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> милл</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t>исекундах</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$C$40:$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Usual</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Optimus (Stream)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$40:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25.169033333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>221.53556666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C6A-46D4-8FA3-E72E958E7901}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1836500703"/>
+        <c:axId val="1444802431"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1836500703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1444802431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1444802431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1836500703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$C$115:$C$147</c:f>
+              <c:strCache>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>Usual</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Optimus (Stream)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$115:$D$147</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>440.57440000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.147800000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>407.4178</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>286.54259999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>345.58659999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>364.52300000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>377.18629999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>408.1694</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>415.90679999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>428.93259999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>433.64709999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>454.58190000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>462.5874</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>457.76609999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>467.89690000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>474.00009999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>474.45269999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>476.02719999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>474.46</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>479.73940000000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>480.20729999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>476.40209999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>475.77979999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>481.5213</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>479.98990000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>483.58340000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>488.98359999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>485.46290000000005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>481.93079999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>489.17720000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>488.79950000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>489.85950000000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>485.4529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-91B8-447E-A401-C95509E4587F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2004431967"/>
+        <c:axId val="1886563039"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2004431967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1886563039"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1886563039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2004431967"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1754,6 +2520,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2761,6 +3607,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3368,6 +5220,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>308161</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>11207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A193F9DF-7C75-47CF-9027-F635E1CDCC90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>604571</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Диаграмма 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DEEDB6F-45DA-48A6-8B90-3ECEB270BFD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3675,17 +5599,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D94D687-82E9-4018-8178-D13A8669E2BA}">
   <dimension ref="B2:AG147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="8" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
@@ -3715,14 +5640,12 @@
       </c>
       <c r="D3" s="10">
         <f>SUM(E3:N3) / COUNT(E3:N3)/ 1000 / 1000</f>
-        <v>23.286999999999999</v>
+        <v>4033.3507999999997</v>
       </c>
       <c r="E3" s="1">
-        <v>23847200</v>
-      </c>
-      <c r="F3" s="1">
-        <v>22726800</v>
-      </c>
+        <v>4033350800</v>
+      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3738,14 +5661,12 @@
       </c>
       <c r="D4" s="10">
         <f t="shared" ref="D4:D35" si="0">SUM(E4:N4) / COUNT(E4:N4)/ 1000 / 1000</f>
-        <v>35.515500000000003</v>
+        <v>2361.6039999999998</v>
       </c>
       <c r="E4" s="1">
-        <v>43068800</v>
-      </c>
-      <c r="F4" s="1">
-        <v>27962200</v>
-      </c>
+        <v>2361604000</v>
+      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3764,14 +5685,12 @@
       </c>
       <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>17.363849999999999</v>
+        <v>4093.4922999999999</v>
       </c>
       <c r="E5" s="1">
-        <v>17070500</v>
-      </c>
-      <c r="F5" s="1">
-        <v>17657200</v>
-      </c>
+        <v>4093492300</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -3788,14 +5707,12 @@
       </c>
       <c r="D6" s="10">
         <f t="shared" si="0"/>
-        <v>45.317999999999998</v>
+        <v>2023.3779</v>
       </c>
       <c r="E6" s="1">
-        <v>34034800</v>
-      </c>
-      <c r="F6" s="1">
-        <v>56601200</v>
-      </c>
+        <v>2023377900</v>
+      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -3812,14 +5729,12 @@
       </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
-        <v>52.698250000000002</v>
+        <v>4467.8284000000003</v>
       </c>
       <c r="E7" s="1">
-        <v>55877500</v>
-      </c>
-      <c r="F7" s="1">
-        <v>49519000</v>
-      </c>
+        <v>4467828400</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -3837,14 +5752,12 @@
       </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
-        <v>41.61795</v>
+        <v>4519.5195999999996</v>
       </c>
       <c r="E8" s="1">
-        <v>38368400</v>
-      </c>
-      <c r="F8" s="1">
-        <v>44867500</v>
-      </c>
+        <v>4519519600</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -3862,14 +5775,12 @@
       </c>
       <c r="D9" s="10">
         <f t="shared" si="0"/>
-        <v>43.782249999999998</v>
+        <v>4636.1889000000001</v>
       </c>
       <c r="E9" s="1">
-        <v>42445500</v>
-      </c>
-      <c r="F9" s="1">
-        <v>45119000</v>
-      </c>
+        <v>4636188900</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -3887,14 +5798,12 @@
       </c>
       <c r="D10" s="10">
         <f t="shared" si="0"/>
-        <v>41.986050000000006</v>
+        <v>4794.2619000000004</v>
       </c>
       <c r="E10" s="1">
-        <v>43871300</v>
-      </c>
-      <c r="F10" s="1">
-        <v>40100800</v>
-      </c>
+        <v>4794261900</v>
+      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -3912,14 +5821,12 @@
       </c>
       <c r="D11" s="10">
         <f t="shared" si="0"/>
-        <v>42.423250000000003</v>
+        <v>5055.3064999999997</v>
       </c>
       <c r="E11" s="1">
-        <v>41498800</v>
-      </c>
-      <c r="F11" s="1">
-        <v>43347700</v>
-      </c>
+        <v>5055306500</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -3937,14 +5844,12 @@
       </c>
       <c r="D12" s="10">
         <f t="shared" si="0"/>
-        <v>43.198250000000002</v>
+        <v>5118.8723</v>
       </c>
       <c r="E12" s="1">
-        <v>42146400</v>
-      </c>
-      <c r="F12" s="1">
-        <v>44250100</v>
-      </c>
+        <v>5118872300</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -3962,14 +5867,12 @@
       </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>37.142400000000002</v>
+        <v>5304.3768</v>
       </c>
       <c r="E13" s="1">
-        <v>38486800</v>
-      </c>
-      <c r="F13" s="1">
-        <v>35798000</v>
-      </c>
+        <v>5304376800</v>
+      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -3987,14 +5890,12 @@
       </c>
       <c r="D14" s="10">
         <f t="shared" si="0"/>
-        <v>40.909550000000003</v>
+        <v>5386.2038000000002</v>
       </c>
       <c r="E14" s="1">
-        <v>43308400</v>
-      </c>
-      <c r="F14" s="1">
-        <v>38510700</v>
-      </c>
+        <v>5386203800</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -4012,14 +5913,12 @@
       </c>
       <c r="D15" s="10">
         <f t="shared" si="0"/>
-        <v>36.543550000000003</v>
+        <v>5461.3427000000001</v>
       </c>
       <c r="E15" s="1">
-        <v>40023400</v>
-      </c>
-      <c r="F15" s="1">
-        <v>33063700</v>
-      </c>
+        <v>5461342700</v>
+      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -4037,14 +5936,12 @@
       </c>
       <c r="D16" s="10">
         <f t="shared" si="0"/>
-        <v>36.555199999999999</v>
+        <v>5596.9142000000002</v>
       </c>
       <c r="E16" s="1">
-        <v>37513500</v>
-      </c>
-      <c r="F16" s="1">
-        <v>35596900</v>
-      </c>
+        <v>5596914200</v>
+      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -4062,14 +5959,12 @@
       </c>
       <c r="D17" s="10">
         <f t="shared" si="0"/>
-        <v>36.462449999999997</v>
+        <v>5718.4560000000001</v>
       </c>
       <c r="E17" s="1">
-        <v>36667300</v>
-      </c>
-      <c r="F17" s="1">
-        <v>36257600</v>
-      </c>
+        <v>5718456000</v>
+      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -4087,14 +5982,12 @@
       </c>
       <c r="D18" s="10">
         <f t="shared" si="0"/>
-        <v>34.431650000000005</v>
+        <v>5848.3908000000001</v>
       </c>
       <c r="E18" s="1">
-        <v>32566000</v>
-      </c>
-      <c r="F18" s="1">
-        <v>36297300</v>
-      </c>
+        <v>5848390800</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -4112,14 +6005,12 @@
       </c>
       <c r="D19" s="10">
         <f t="shared" si="0"/>
-        <v>33.344149999999999</v>
+        <v>5888.8244999999997</v>
       </c>
       <c r="E19" s="1">
-        <v>30773800</v>
-      </c>
-      <c r="F19" s="1">
-        <v>35914500</v>
-      </c>
+        <v>5888824500</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -4137,14 +6028,12 @@
       </c>
       <c r="D20" s="10">
         <f t="shared" si="0"/>
-        <v>32.16545</v>
+        <v>5869.1355999999996</v>
       </c>
       <c r="E20" s="1">
-        <v>31039200</v>
-      </c>
-      <c r="F20" s="1">
-        <v>33291700</v>
-      </c>
+        <v>5869135600</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -4162,14 +6051,12 @@
       </c>
       <c r="D21" s="10">
         <f t="shared" si="0"/>
-        <v>32.469349999999999</v>
+        <v>5891.8882000000003</v>
       </c>
       <c r="E21" s="1">
-        <v>30610500</v>
-      </c>
-      <c r="F21" s="1">
-        <v>34328200</v>
-      </c>
+        <v>5891888200</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -4187,14 +6074,12 @@
       </c>
       <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>33.022150000000003</v>
+        <v>5939.5755999999992</v>
       </c>
       <c r="E22" s="1">
-        <v>31587900</v>
-      </c>
-      <c r="F22" s="1">
-        <v>34456400</v>
-      </c>
+        <v>5939575600</v>
+      </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -4212,14 +6097,12 @@
       </c>
       <c r="D23" s="10">
         <f t="shared" si="0"/>
-        <v>33.774149999999999</v>
+        <v>5869.9935999999998</v>
       </c>
       <c r="E23" s="1">
-        <v>32468900</v>
-      </c>
-      <c r="F23" s="1">
-        <v>35079400</v>
-      </c>
+        <v>5869993600</v>
+      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -4237,14 +6120,12 @@
       </c>
       <c r="D24" s="10">
         <f t="shared" si="0"/>
-        <v>32.425849999999997</v>
+        <v>6478.9552999999996</v>
       </c>
       <c r="E24" s="1">
-        <v>32034500</v>
-      </c>
-      <c r="F24" s="1">
-        <v>32817200</v>
-      </c>
+        <v>6478955300</v>
+      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -4262,14 +6143,12 @@
       </c>
       <c r="D25" s="10">
         <f t="shared" si="0"/>
-        <v>33.772599999999997</v>
+        <v>6675.9492</v>
       </c>
       <c r="E25" s="1">
-        <v>33594600</v>
-      </c>
-      <c r="F25" s="1">
-        <v>33950600</v>
-      </c>
+        <v>6675949200</v>
+      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -4287,14 +6166,12 @@
       </c>
       <c r="D26" s="10">
         <f t="shared" si="0"/>
-        <v>35.000599999999999</v>
+        <v>6655.8872999999994</v>
       </c>
       <c r="E26" s="1">
-        <v>33151000</v>
-      </c>
-      <c r="F26" s="1">
-        <v>36850200</v>
-      </c>
+        <v>6655887300</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -4312,14 +6189,12 @@
       </c>
       <c r="D27" s="10">
         <f t="shared" si="0"/>
-        <v>34.5334</v>
+        <v>6223.5045</v>
       </c>
       <c r="E27" s="1">
-        <v>31464400</v>
-      </c>
-      <c r="F27" s="1">
-        <v>37602400</v>
-      </c>
+        <v>6223504500</v>
+      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -4337,14 +6212,12 @@
       </c>
       <c r="D28" s="10">
         <f t="shared" si="0"/>
-        <v>34.182250000000003</v>
+        <v>5958.7987999999996</v>
       </c>
       <c r="E28" s="1">
-        <v>31338000</v>
-      </c>
-      <c r="F28" s="1">
-        <v>37026500</v>
-      </c>
+        <v>5958798800</v>
+      </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -4362,14 +6235,12 @@
       </c>
       <c r="D29" s="10">
         <f t="shared" si="0"/>
-        <v>32.964150000000004</v>
+        <v>5958.3064999999997</v>
       </c>
       <c r="E29" s="1">
-        <v>33178300</v>
-      </c>
-      <c r="F29" s="1">
-        <v>32750000</v>
-      </c>
+        <v>5958306500</v>
+      </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -4387,14 +6258,12 @@
       </c>
       <c r="D30" s="10">
         <f t="shared" si="0"/>
-        <v>35.02225</v>
+        <v>5965.9070999999994</v>
       </c>
       <c r="E30" s="1">
-        <v>33487600</v>
-      </c>
-      <c r="F30" s="1">
-        <v>36556900</v>
-      </c>
+        <v>5965907100</v>
+      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -4412,14 +6281,12 @@
       </c>
       <c r="D31" s="10">
         <f t="shared" si="0"/>
-        <v>33.097749999999998</v>
+        <v>5958.8387000000002</v>
       </c>
       <c r="E31" s="1">
-        <v>30722200</v>
-      </c>
-      <c r="F31" s="1">
-        <v>35473300</v>
-      </c>
+        <v>5958838700</v>
+      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -4437,14 +6304,12 @@
       </c>
       <c r="D32" s="10">
         <f t="shared" si="0"/>
-        <v>32.353650000000002</v>
+        <v>5962.8292999999994</v>
       </c>
       <c r="E32" s="1">
-        <v>30693000</v>
-      </c>
-      <c r="F32" s="1">
-        <v>34014300</v>
-      </c>
+        <v>5962829300</v>
+      </c>
+      <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -4462,14 +6327,12 @@
       </c>
       <c r="D33" s="10">
         <f t="shared" si="0"/>
-        <v>33.407849999999996</v>
+        <v>5986.7290000000003</v>
       </c>
       <c r="E33" s="1">
-        <v>32195000</v>
-      </c>
-      <c r="F33" s="1">
-        <v>34620700</v>
-      </c>
+        <v>5986729000</v>
+      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -4487,14 +6350,12 @@
       </c>
       <c r="D34" s="10">
         <f t="shared" si="0"/>
-        <v>30.833200000000001</v>
+        <v>5987.3458000000001</v>
       </c>
       <c r="E34" s="1">
-        <v>30919500</v>
-      </c>
-      <c r="F34" s="1">
-        <v>30746900</v>
-      </c>
+        <v>5987345800</v>
+      </c>
+      <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -4512,14 +6373,12 @@
       </c>
       <c r="D35" s="10">
         <f t="shared" si="0"/>
-        <v>31.266349999999999</v>
+        <v>5979.7764999999999</v>
       </c>
       <c r="E35" s="1">
-        <v>30731800</v>
-      </c>
-      <c r="F35" s="1">
-        <v>31800900</v>
-      </c>
+        <v>5979776500</v>
+      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -4556,27 +6415,26 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="40" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1</v>
+      </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="5">
-        <f>SUM(E40:N40) / COUNT(E40:N40)/ 1000 / 1000</f>
-        <v>33.545449999999995</v>
+        <f>SUM(E40:N40) / COUNT(E40:N40)/ 1000 / 1000 / B40</f>
+        <v>25.169033333333331</v>
       </c>
       <c r="E40" s="1">
-        <v>28433300</v>
-      </c>
-      <c r="F40" s="1">
-        <v>47469700</v>
+        <v>25651700</v>
+      </c>
+      <c r="F40" s="13">
+        <v>24927700</v>
       </c>
       <c r="G40" s="1">
-        <f>AG40/10</f>
-        <v>24733350</v>
+        <v>24927700</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -4590,22 +6448,24 @@
       </c>
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1</v>
+      </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" ref="D41:D72" si="1">SUM(E41:N41) / COUNT(E41:N41)/ 1000 / 1000</f>
-        <v>102.09437333333332</v>
+        <f>SUM(E41:N41) / COUNT(E41:N41)/ 1000 / 1000 / B41</f>
+        <v>221.53556666666665</v>
       </c>
       <c r="E41" s="1">
-        <v>49979400</v>
+        <v>219793300</v>
       </c>
       <c r="F41" s="1">
-        <v>52847000</v>
+        <v>222406700</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" ref="G41:G72" si="2">AG41/10</f>
-        <v>203456720</v>
+        <v>222406700</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -4626,18 +6486,17 @@
         <v>1</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="1"/>
-        <v>31.84225</v>
+        <f t="shared" ref="D42:D72" si="1">SUM(E42:N42) / COUNT(E42:N42)/ 1000 / 1000</f>
+        <v>0.36516666666666669</v>
       </c>
       <c r="E42" s="1">
-        <v>32539000</v>
+        <v>334300</v>
       </c>
       <c r="F42" s="1">
-        <v>39680700</v>
+        <v>380600</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" si="2"/>
-        <v>23307050</v>
+        <v>380600</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -4657,17 +6516,16 @@
       </c>
       <c r="D43" s="5">
         <f t="shared" si="1"/>
-        <v>286.87023999999997</v>
+        <v>0.33176666666666671</v>
       </c>
       <c r="E43" s="1">
-        <v>244041400</v>
+        <v>345300</v>
       </c>
       <c r="F43" s="1">
-        <v>300531500</v>
+        <v>325000</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" si="2"/>
-        <v>316037820</v>
+        <v>325000</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -4687,17 +6545,16 @@
       </c>
       <c r="D44" s="5">
         <f t="shared" si="1"/>
-        <v>354.46147333333334</v>
+        <v>0.4088</v>
       </c>
       <c r="E44" s="1">
-        <v>357423100</v>
+        <v>343600</v>
       </c>
       <c r="F44" s="1">
-        <v>331776400</v>
+        <v>441400</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" si="2"/>
-        <v>374184920</v>
+        <v>441400</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -4717,17 +6574,16 @@
       </c>
       <c r="D45" s="5">
         <f t="shared" si="1"/>
-        <v>377.6347566666667</v>
+        <v>0.4234</v>
       </c>
       <c r="E45" s="1">
-        <v>345213600</v>
+        <v>404600</v>
       </c>
       <c r="F45" s="1">
-        <v>361984100</v>
+        <v>432800</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="2"/>
-        <v>425706570</v>
+        <v>432800</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -4747,17 +6603,16 @@
       </c>
       <c r="D46" s="5">
         <f t="shared" si="1"/>
-        <v>433.45422333333335</v>
+        <v>0.4264</v>
       </c>
       <c r="E46" s="1">
-        <v>409804400</v>
+        <v>350200</v>
       </c>
       <c r="F46" s="1">
-        <v>400214900</v>
+        <v>464500</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" si="2"/>
-        <v>490343370</v>
+        <v>464500</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -4777,17 +6632,16 @@
       </c>
       <c r="D47" s="5">
         <f t="shared" si="1"/>
-        <v>437.4499633333333</v>
+        <v>0.435</v>
       </c>
       <c r="E47" s="1">
-        <v>430005300</v>
+        <v>502600</v>
       </c>
       <c r="F47" s="1">
-        <v>397526700</v>
+        <v>401200</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="2"/>
-        <v>484817890</v>
+        <v>401200</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -4807,17 +6661,16 @@
       </c>
       <c r="D48" s="5">
         <f t="shared" si="1"/>
-        <v>410.13909666666666</v>
+        <v>0.43969999999999998</v>
       </c>
       <c r="E48" s="1">
-        <v>361169300</v>
+        <v>430900</v>
       </c>
       <c r="F48" s="1">
-        <v>396955300</v>
+        <v>444100</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" si="2"/>
-        <v>472292690</v>
+        <v>444100</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -4837,17 +6690,16 @@
       </c>
       <c r="D49" s="5">
         <f t="shared" si="1"/>
-        <v>403.21022999999997</v>
+        <v>0.55210000000000004</v>
       </c>
       <c r="E49" s="1">
-        <v>356284800</v>
+        <v>581700</v>
       </c>
       <c r="F49" s="1">
-        <v>369938800</v>
+        <v>537300</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="2"/>
-        <v>483407090</v>
+        <v>537300</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -4867,17 +6719,16 @@
       </c>
       <c r="D50" s="5">
         <f t="shared" si="1"/>
-        <v>422.72969333333327</v>
+        <v>0.56720000000000004</v>
       </c>
       <c r="E50" s="1">
-        <v>373302800</v>
+        <v>582600</v>
       </c>
       <c r="F50" s="1">
-        <v>394570600</v>
+        <v>559500</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="2"/>
-        <v>500315680</v>
+        <v>559500</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -4897,17 +6748,16 @@
       </c>
       <c r="D51" s="5">
         <f t="shared" si="1"/>
-        <v>408.34453999999999</v>
+        <v>0.60363333333333336</v>
       </c>
       <c r="E51" s="1">
-        <v>366315400</v>
+        <v>622300</v>
       </c>
       <c r="F51" s="1">
-        <v>368913500</v>
+        <v>594300</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="2"/>
-        <v>489804720</v>
+        <v>594300</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -4927,17 +6777,16 @@
       </c>
       <c r="D52" s="5">
         <f t="shared" si="1"/>
-        <v>382.1543733333333</v>
+        <v>0.64136666666666664</v>
       </c>
       <c r="E52" s="1">
-        <v>328730900</v>
+        <v>683100</v>
       </c>
       <c r="F52" s="1">
-        <v>362363700</v>
+        <v>620500</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="2"/>
-        <v>455368520</v>
+        <v>620500</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -4957,17 +6806,16 @@
       </c>
       <c r="D53" s="5">
         <f t="shared" si="1"/>
-        <v>373.7577766666667</v>
+        <v>0.69653333333333345</v>
       </c>
       <c r="E53" s="1">
-        <v>332586300</v>
+        <v>719000</v>
       </c>
       <c r="F53" s="1">
-        <v>350982800</v>
+        <v>685300</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="2"/>
-        <v>437704230</v>
+        <v>685300</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -4987,17 +6835,16 @@
       </c>
       <c r="D54" s="5">
         <f t="shared" si="1"/>
-        <v>349.93829333333332</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="E54" s="1">
-        <v>316142600</v>
+        <v>753400</v>
       </c>
       <c r="F54" s="1">
-        <v>332955200</v>
+        <v>730300</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="2"/>
-        <v>400717080</v>
+        <v>730300</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -5017,17 +6864,16 @@
       </c>
       <c r="D55" s="5">
         <f t="shared" si="1"/>
-        <v>349.15191666666669</v>
+        <v>1.2566666666666668</v>
       </c>
       <c r="E55" s="1">
-        <v>329674800</v>
+        <v>830800</v>
       </c>
       <c r="F55" s="1">
-        <v>330660700</v>
+        <v>1469600</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" si="2"/>
-        <v>387120250</v>
+        <v>1469600</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -5047,17 +6893,16 @@
       </c>
       <c r="D56" s="5">
         <f t="shared" si="1"/>
-        <v>334.30834999999996</v>
+        <v>0.82023333333333337</v>
       </c>
       <c r="E56" s="1">
-        <v>311630700</v>
+        <v>791900</v>
       </c>
       <c r="F56" s="1">
-        <v>319788100</v>
+        <v>834400</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="2"/>
-        <v>371506250</v>
+        <v>834400</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -5077,17 +6922,16 @@
       </c>
       <c r="D57" s="5">
         <f t="shared" si="1"/>
-        <v>320.80375666666669</v>
+        <v>0.84033333333333338</v>
       </c>
       <c r="E57" s="1">
-        <v>304338000</v>
+        <v>864200</v>
       </c>
       <c r="F57" s="1">
-        <v>305499100</v>
+        <v>828400</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="2"/>
-        <v>352574170</v>
+        <v>828400</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -5107,17 +6951,16 @@
       </c>
       <c r="D58" s="5">
         <f t="shared" si="1"/>
-        <v>330.76777000000004</v>
+        <v>0.95563333333333333</v>
       </c>
       <c r="E58" s="1">
-        <v>316924000</v>
+        <v>973300</v>
       </c>
       <c r="F58" s="1">
-        <v>310097300</v>
+        <v>946800</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="2"/>
-        <v>365282010</v>
+        <v>946800</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -5137,17 +6980,16 @@
       </c>
       <c r="D59" s="5">
         <f t="shared" si="1"/>
-        <v>329.44851</v>
+        <v>1.7404999999999999</v>
       </c>
       <c r="E59" s="1">
-        <v>300466100</v>
+        <v>1177300</v>
       </c>
       <c r="F59" s="1">
-        <v>312368400</v>
+        <v>2022100</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="2"/>
-        <v>375511030</v>
+        <v>2022100</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -5167,17 +7009,16 @@
       </c>
       <c r="D60" s="5">
         <f t="shared" si="1"/>
-        <v>318.64961999999997</v>
+        <v>2.1255666666666668</v>
       </c>
       <c r="E60" s="1">
-        <v>303160700</v>
+        <v>1059500</v>
       </c>
       <c r="F60" s="1">
-        <v>301508200</v>
+        <v>2658600</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="2"/>
-        <v>351279960</v>
+        <v>2658600</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -5197,17 +7038,16 @@
       </c>
       <c r="D61" s="5">
         <f t="shared" si="1"/>
-        <v>316.99907000000002</v>
+        <v>1.2076333333333331</v>
       </c>
       <c r="E61" s="1">
-        <v>297279900</v>
+        <v>1070900</v>
       </c>
       <c r="F61" s="1">
-        <v>296456600</v>
+        <v>1276000</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" si="2"/>
-        <v>357260710</v>
+        <v>1276000</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -5227,17 +7067,16 @@
       </c>
       <c r="D62" s="5">
         <f t="shared" si="1"/>
-        <v>313.93516999999997</v>
+        <v>2.4201333333333337</v>
       </c>
       <c r="E62" s="1">
-        <v>304024900</v>
+        <v>1390200</v>
       </c>
       <c r="F62" s="1">
-        <v>297238300</v>
+        <v>2935100</v>
       </c>
       <c r="G62" s="1">
-        <f t="shared" si="2"/>
-        <v>340542310</v>
+        <v>2935100</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -5257,17 +7096,16 @@
       </c>
       <c r="D63" s="5">
         <f t="shared" si="1"/>
-        <v>326.15464666666668</v>
+        <v>1.5143333333333333</v>
       </c>
       <c r="E63" s="1">
-        <v>302677200</v>
+        <v>1280400</v>
       </c>
       <c r="F63" s="1">
-        <v>312758700</v>
+        <v>1631300</v>
       </c>
       <c r="G63" s="1">
-        <f t="shared" si="2"/>
-        <v>363028040</v>
+        <v>1631300</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -5287,17 +7125,16 @@
       </c>
       <c r="D64" s="5">
         <f t="shared" si="1"/>
-        <v>317.04913666666664</v>
+        <v>1.5115666666666667</v>
       </c>
       <c r="E64" s="1">
-        <v>297965800</v>
+        <v>1389500</v>
       </c>
       <c r="F64" s="1">
-        <v>303472000</v>
+        <v>1572600</v>
       </c>
       <c r="G64" s="1">
-        <f t="shared" si="2"/>
-        <v>349709610</v>
+        <v>1572600</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -5317,17 +7154,16 @@
       </c>
       <c r="D65" s="5">
         <f t="shared" si="1"/>
-        <v>322.84330666666671</v>
+        <v>1.2510999999999999</v>
       </c>
       <c r="E65" s="1">
-        <v>309177100</v>
+        <v>1167500</v>
       </c>
       <c r="F65" s="1">
-        <v>313048000</v>
+        <v>1292900</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" si="2"/>
-        <v>346304820</v>
+        <v>1292900</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -5347,17 +7183,16 @@
       </c>
       <c r="D66" s="5">
         <f t="shared" si="1"/>
-        <v>362.56063666666665</v>
+        <v>1.3248333333333333</v>
       </c>
       <c r="E66" s="1">
-        <v>303775000</v>
+        <v>1325300</v>
       </c>
       <c r="F66" s="1">
-        <v>431818300</v>
+        <v>1324600</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" si="2"/>
-        <v>352088610</v>
+        <v>1324600</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -5377,17 +7212,16 @@
       </c>
       <c r="D67" s="5">
         <f t="shared" si="1"/>
-        <v>327.00149333333331</v>
+        <v>1.5193666666666668</v>
       </c>
       <c r="E67" s="1">
-        <v>313496500</v>
+        <v>1592100</v>
       </c>
       <c r="F67" s="1">
-        <v>322596400</v>
+        <v>1483000</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" si="2"/>
-        <v>344911580</v>
+        <v>1483000</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -5407,17 +7241,16 @@
       </c>
       <c r="D68" s="5">
         <f t="shared" si="1"/>
-        <v>318.19207333333333</v>
+        <v>1.7243666666666668</v>
       </c>
       <c r="E68" s="1">
-        <v>299808300</v>
+        <v>2038100</v>
       </c>
       <c r="F68" s="1">
-        <v>306056000</v>
+        <v>1567500</v>
       </c>
       <c r="G68" s="1">
-        <f t="shared" si="2"/>
-        <v>348711920</v>
+        <v>1567500</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -5437,17 +7270,16 @@
       </c>
       <c r="D69" s="5">
         <f t="shared" si="1"/>
-        <v>328.18165000000005</v>
+        <v>1.4458666666666669</v>
       </c>
       <c r="E69" s="1">
-        <v>313287100</v>
+        <v>1583600</v>
       </c>
       <c r="F69" s="1">
-        <v>326549700</v>
+        <v>1377000</v>
       </c>
       <c r="G69" s="1">
-        <f t="shared" si="2"/>
-        <v>344708150</v>
+        <v>1377000</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
@@ -5467,17 +7299,16 @@
       </c>
       <c r="D70" s="5">
         <f t="shared" si="1"/>
-        <v>360.72090999999995</v>
+        <v>1.4727666666666666</v>
       </c>
       <c r="E70" s="1">
-        <v>304203800</v>
+        <v>1738500</v>
       </c>
       <c r="F70" s="1">
-        <v>426975400</v>
+        <v>1339900</v>
       </c>
       <c r="G70" s="1">
-        <f t="shared" si="2"/>
-        <v>350983530</v>
+        <v>1339900</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
@@ -5497,17 +7328,16 @@
       </c>
       <c r="D71" s="5">
         <f t="shared" si="1"/>
-        <v>360.95258000000001</v>
+        <v>1.4951333333333332</v>
       </c>
       <c r="E71" s="1">
-        <v>306587100</v>
+        <v>1692600</v>
       </c>
       <c r="F71" s="1">
-        <v>417802500</v>
+        <v>1396400</v>
       </c>
       <c r="G71" s="1">
-        <f t="shared" si="2"/>
-        <v>358468140</v>
+        <v>1396400</v>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
@@ -5527,17 +7357,16 @@
       </c>
       <c r="D72" s="5">
         <f t="shared" si="1"/>
-        <v>342.80452000000002</v>
+        <v>1.6969333333333332</v>
       </c>
       <c r="E72" s="1">
-        <v>304619800</v>
+        <v>1838800</v>
       </c>
       <c r="F72" s="1">
-        <v>364964000</v>
+        <v>1626000</v>
       </c>
       <c r="G72" s="1">
-        <f t="shared" si="2"/>
-        <v>358829760</v>
+        <v>1626000</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
@@ -5607,7 +7436,7 @@
         <v>2</v>
       </c>
       <c r="D78" s="5">
-        <f t="shared" ref="D78:D109" si="3">SUM(E78:N78) / COUNT(E78:N78)/ 1000 / 1000</f>
+        <f t="shared" ref="D78:D109" si="2">SUM(E78:N78) / COUNT(E78:N78)/ 1000 / 1000</f>
         <v>968.4126</v>
       </c>
       <c r="E78" s="1">
@@ -5637,7 +7466,7 @@
         <v>1</v>
       </c>
       <c r="D79" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>220.41729999999998</v>
       </c>
       <c r="E79" s="1">
@@ -5665,7 +7494,7 @@
         <v>2</v>
       </c>
       <c r="D80" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2520.1049750000002</v>
       </c>
       <c r="E80" s="1">
@@ -5693,7 +7522,7 @@
         <v>3</v>
       </c>
       <c r="D81" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3125.7725</v>
       </c>
       <c r="E81" s="1">
@@ -5721,7 +7550,7 @@
         <v>4</v>
       </c>
       <c r="D82" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3732.9300750000002</v>
       </c>
       <c r="E82" s="1">
@@ -5749,7 +7578,7 @@
         <v>5</v>
       </c>
       <c r="D83" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3659.3316500000001</v>
       </c>
       <c r="E83" s="1">
@@ -5777,7 +7606,7 @@
         <v>6</v>
       </c>
       <c r="D84" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3422.7775499999998</v>
       </c>
       <c r="E84" s="1">
@@ -5805,7 +7634,7 @@
         <v>7</v>
       </c>
       <c r="D85" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3099.3313750000002</v>
       </c>
       <c r="E85" s="1">
@@ -5833,7 +7662,7 @@
         <v>8</v>
       </c>
       <c r="D86" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3121.9437749999997</v>
       </c>
       <c r="E86" s="1">
@@ -5861,7 +7690,7 @@
         <v>9</v>
       </c>
       <c r="D87" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3171.8808749999998</v>
       </c>
       <c r="E87" s="1">
@@ -5889,7 +7718,7 @@
         <v>10</v>
       </c>
       <c r="D88" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3155.7731749999998</v>
       </c>
       <c r="E88" s="1">
@@ -5917,7 +7746,7 @@
         <v>11</v>
       </c>
       <c r="D89" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3163.0625249999998</v>
       </c>
       <c r="E89" s="1">
@@ -5945,7 +7774,7 @@
         <v>12</v>
       </c>
       <c r="D90" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3258.3580499999998</v>
       </c>
       <c r="E90" s="1">
@@ -5973,7 +7802,7 @@
         <v>13</v>
       </c>
       <c r="D91" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3264.6103499999999</v>
       </c>
       <c r="E91" s="1">
@@ -6001,7 +7830,7 @@
         <v>14</v>
       </c>
       <c r="D92" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3187.1091499999998</v>
       </c>
       <c r="E92" s="1">
@@ -6029,7 +7858,7 @@
         <v>15</v>
       </c>
       <c r="D93" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3352.389525</v>
       </c>
       <c r="E93" s="1">
@@ -6057,7 +7886,7 @@
         <v>16</v>
       </c>
       <c r="D94" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3198.14455</v>
       </c>
       <c r="E94" s="1">
@@ -6085,7 +7914,7 @@
         <v>17</v>
       </c>
       <c r="D95" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3168.8187749999997</v>
       </c>
       <c r="E95" s="1">
@@ -6113,7 +7942,7 @@
         <v>18</v>
       </c>
       <c r="D96" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3163.9285249999998</v>
       </c>
       <c r="E96" s="1">
@@ -6141,7 +7970,7 @@
         <v>19</v>
       </c>
       <c r="D97" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3142.725375</v>
       </c>
       <c r="E97" s="1">
@@ -6169,7 +7998,7 @@
         <v>20</v>
       </c>
       <c r="D98" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3241.3328999999999</v>
       </c>
       <c r="E98" s="1">
@@ -6197,7 +8026,7 @@
         <v>21</v>
       </c>
       <c r="D99" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3198.67355</v>
       </c>
       <c r="E99" s="1">
@@ -6225,7 +8054,7 @@
         <v>22</v>
       </c>
       <c r="D100" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3290.8587000000002</v>
       </c>
       <c r="E100" s="1">
@@ -6253,7 +8082,7 @@
         <v>23</v>
       </c>
       <c r="D101" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3143.5763999999999</v>
       </c>
       <c r="E101" s="1">
@@ -6281,7 +8110,7 @@
         <v>24</v>
       </c>
       <c r="D102" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2768.4515499999998</v>
       </c>
       <c r="E102" s="1">
@@ -6309,7 +8138,7 @@
         <v>25</v>
       </c>
       <c r="D103" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2509.0195750000003</v>
       </c>
       <c r="E103" s="1">
@@ -6337,7 +8166,7 @@
         <v>26</v>
       </c>
       <c r="D104" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2572.3301749999996</v>
       </c>
       <c r="E104" s="1">
@@ -6365,7 +8194,7 @@
         <v>27</v>
       </c>
       <c r="D105" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2580.5604500000004</v>
       </c>
       <c r="E105" s="1">
@@ -6393,7 +8222,7 @@
         <v>28</v>
       </c>
       <c r="D106" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2763.2431499999998</v>
       </c>
       <c r="E106" s="1">
@@ -6421,7 +8250,7 @@
         <v>29</v>
       </c>
       <c r="D107" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3042.1008500000003</v>
       </c>
       <c r="E107" s="1">
@@ -6449,7 +8278,7 @@
         <v>30</v>
       </c>
       <c r="D108" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3287.0614500000001</v>
       </c>
       <c r="E108" s="1">
@@ -6477,7 +8306,7 @@
         <v>31</v>
       </c>
       <c r="D109" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3291.7092000000002</v>
       </c>
       <c r="E109" s="1">
@@ -6499,98 +8328,445 @@
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E117" s="8"/>
-    </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E118" s="8"/>
-    </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E119" s="8"/>
-    </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E120" s="8"/>
-    </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E121" s="8"/>
-    </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E122" s="8"/>
-    </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E123" s="8"/>
-    </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E124" s="8"/>
-    </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E125" s="8"/>
-    </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E126" s="8"/>
-    </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E127" s="8"/>
-    </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E128" s="8"/>
-    </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E129" s="8"/>
-    </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E130" s="8"/>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E131" s="8"/>
-    </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E132" s="8"/>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E133" s="8"/>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E134" s="8"/>
-    </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E135" s="8"/>
-    </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E136" s="8"/>
-    </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E137" s="8"/>
-    </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E138" s="8"/>
-    </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E139" s="8"/>
-    </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E140" s="9"/>
-    </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E141" s="9"/>
-    </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E142" s="9"/>
-    </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E143" s="9"/>
-    </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E144" s="9"/>
-    </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E145" s="9"/>
-    </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E146" s="9"/>
-    </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E147" s="9"/>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>0</v>
+      </c>
+      <c r="D115" s="5">
+        <f>SUM(E115:N115) / COUNT(E115:N115)/ 1000 / 1000</f>
+        <v>440.57440000000003</v>
+      </c>
+      <c r="E115">
+        <v>440574400</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D116" s="5">
+        <f t="shared" ref="D116:D147" si="3">SUM(E116:N116) / COUNT(E116:N116)/ 1000 / 1000</f>
+        <v>72.147800000000004</v>
+      </c>
+      <c r="E116">
+        <v>72147800</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" s="7">
+        <v>1</v>
+      </c>
+      <c r="D117" s="5">
+        <f t="shared" si="3"/>
+        <v>407.4178</v>
+      </c>
+      <c r="E117">
+        <v>407417800</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="6"/>
+      <c r="C118" s="7">
+        <v>2</v>
+      </c>
+      <c r="D118" s="5">
+        <f t="shared" si="3"/>
+        <v>286.54259999999999</v>
+      </c>
+      <c r="E118">
+        <v>286542600</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B119" s="6"/>
+      <c r="C119" s="7">
+        <v>3</v>
+      </c>
+      <c r="D119" s="5">
+        <f t="shared" si="3"/>
+        <v>345.58659999999998</v>
+      </c>
+      <c r="E119">
+        <v>345586600</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B120" s="6"/>
+      <c r="C120" s="7">
+        <v>4</v>
+      </c>
+      <c r="D120" s="5">
+        <f t="shared" si="3"/>
+        <v>364.52300000000002</v>
+      </c>
+      <c r="E120">
+        <v>364523000</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B121" s="6"/>
+      <c r="C121" s="7">
+        <v>5</v>
+      </c>
+      <c r="D121" s="5">
+        <f t="shared" si="3"/>
+        <v>377.18629999999996</v>
+      </c>
+      <c r="E121">
+        <v>377186300</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B122" s="6"/>
+      <c r="C122" s="7">
+        <v>6</v>
+      </c>
+      <c r="D122" s="5">
+        <f t="shared" si="3"/>
+        <v>408.1694</v>
+      </c>
+      <c r="E122">
+        <v>408169400</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B123" s="6"/>
+      <c r="C123" s="7">
+        <v>7</v>
+      </c>
+      <c r="D123" s="5">
+        <f t="shared" si="3"/>
+        <v>415.90679999999998</v>
+      </c>
+      <c r="E123">
+        <v>415906800</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B124" s="6"/>
+      <c r="C124" s="7">
+        <v>8</v>
+      </c>
+      <c r="D124" s="5">
+        <f t="shared" si="3"/>
+        <v>428.93259999999998</v>
+      </c>
+      <c r="E124">
+        <v>428932600</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125" s="6"/>
+      <c r="C125" s="7">
+        <v>9</v>
+      </c>
+      <c r="D125" s="5">
+        <f t="shared" si="3"/>
+        <v>433.64709999999997</v>
+      </c>
+      <c r="E125">
+        <v>433647100</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B126" s="6"/>
+      <c r="C126" s="7">
+        <v>10</v>
+      </c>
+      <c r="D126" s="5">
+        <f t="shared" si="3"/>
+        <v>454.58190000000002</v>
+      </c>
+      <c r="E126">
+        <v>454581900</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127" s="6"/>
+      <c r="C127" s="7">
+        <v>11</v>
+      </c>
+      <c r="D127" s="5">
+        <f t="shared" si="3"/>
+        <v>462.5874</v>
+      </c>
+      <c r="E127">
+        <v>462587400</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B128" s="6"/>
+      <c r="C128" s="7">
+        <v>12</v>
+      </c>
+      <c r="D128" s="5">
+        <f t="shared" si="3"/>
+        <v>457.76609999999999</v>
+      </c>
+      <c r="E128">
+        <v>457766100</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129" s="6"/>
+      <c r="C129" s="7">
+        <v>13</v>
+      </c>
+      <c r="D129" s="5">
+        <f t="shared" si="3"/>
+        <v>467.89690000000002</v>
+      </c>
+      <c r="E129">
+        <v>467896900</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130" s="6"/>
+      <c r="C130" s="7">
+        <v>14</v>
+      </c>
+      <c r="D130" s="5">
+        <f t="shared" si="3"/>
+        <v>474.00009999999997</v>
+      </c>
+      <c r="E130">
+        <v>474000100</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="6"/>
+      <c r="C131" s="7">
+        <v>15</v>
+      </c>
+      <c r="D131" s="5">
+        <f t="shared" si="3"/>
+        <v>474.45269999999999</v>
+      </c>
+      <c r="E131">
+        <v>474452700</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="6"/>
+      <c r="C132" s="7">
+        <v>16</v>
+      </c>
+      <c r="D132" s="5">
+        <f t="shared" si="3"/>
+        <v>476.02719999999999</v>
+      </c>
+      <c r="E132">
+        <v>476027200</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="6"/>
+      <c r="C133" s="7">
+        <v>17</v>
+      </c>
+      <c r="D133" s="5">
+        <f t="shared" si="3"/>
+        <v>474.46</v>
+      </c>
+      <c r="E133">
+        <v>474460000</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134" s="6"/>
+      <c r="C134" s="7">
+        <v>18</v>
+      </c>
+      <c r="D134" s="5">
+        <f t="shared" si="3"/>
+        <v>479.73940000000005</v>
+      </c>
+      <c r="E134">
+        <v>479739400</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135" s="6"/>
+      <c r="C135" s="7">
+        <v>19</v>
+      </c>
+      <c r="D135" s="5">
+        <f t="shared" si="3"/>
+        <v>480.20729999999998</v>
+      </c>
+      <c r="E135">
+        <v>480207300</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B136" s="6"/>
+      <c r="C136" s="7">
+        <v>20</v>
+      </c>
+      <c r="D136" s="5">
+        <f t="shared" si="3"/>
+        <v>476.40209999999996</v>
+      </c>
+      <c r="E136">
+        <v>476402100</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B137" s="6"/>
+      <c r="C137" s="7">
+        <v>21</v>
+      </c>
+      <c r="D137" s="5">
+        <f t="shared" si="3"/>
+        <v>475.77979999999997</v>
+      </c>
+      <c r="E137">
+        <v>475779800</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="6"/>
+      <c r="C138" s="7">
+        <v>22</v>
+      </c>
+      <c r="D138" s="5">
+        <f t="shared" si="3"/>
+        <v>481.5213</v>
+      </c>
+      <c r="E138">
+        <v>481521300</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B139" s="6"/>
+      <c r="C139" s="7">
+        <v>23</v>
+      </c>
+      <c r="D139" s="5">
+        <f t="shared" si="3"/>
+        <v>479.98990000000003</v>
+      </c>
+      <c r="E139">
+        <v>479989900</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B140" s="6"/>
+      <c r="C140" s="7">
+        <v>24</v>
+      </c>
+      <c r="D140" s="5">
+        <f t="shared" si="3"/>
+        <v>483.58340000000004</v>
+      </c>
+      <c r="E140">
+        <v>483583400</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B141" s="6"/>
+      <c r="C141" s="7">
+        <v>25</v>
+      </c>
+      <c r="D141" s="5">
+        <f t="shared" si="3"/>
+        <v>488.98359999999997</v>
+      </c>
+      <c r="E141">
+        <v>488983600</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B142" s="6"/>
+      <c r="C142" s="7">
+        <v>26</v>
+      </c>
+      <c r="D142" s="5">
+        <f t="shared" si="3"/>
+        <v>485.46290000000005</v>
+      </c>
+      <c r="E142">
+        <v>485462900</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B143" s="6"/>
+      <c r="C143" s="7">
+        <v>27</v>
+      </c>
+      <c r="D143" s="5">
+        <f t="shared" si="3"/>
+        <v>481.93079999999998</v>
+      </c>
+      <c r="E143">
+        <v>481930800</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B144" s="6"/>
+      <c r="C144" s="7">
+        <v>28</v>
+      </c>
+      <c r="D144" s="5">
+        <f t="shared" si="3"/>
+        <v>489.17720000000003</v>
+      </c>
+      <c r="E144">
+        <v>489177200</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B145" s="6"/>
+      <c r="C145" s="7">
+        <v>29</v>
+      </c>
+      <c r="D145" s="5">
+        <f t="shared" si="3"/>
+        <v>488.79950000000002</v>
+      </c>
+      <c r="E145">
+        <v>488799500</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="6"/>
+      <c r="C146" s="7">
+        <v>30</v>
+      </c>
+      <c r="D146" s="5">
+        <f t="shared" si="3"/>
+        <v>489.85950000000003</v>
+      </c>
+      <c r="E146">
+        <v>489859500</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="6"/>
+      <c r="C147" s="7">
+        <v>31</v>
+      </c>
+      <c r="D147" s="5">
+        <f t="shared" si="3"/>
+        <v>485.4529</v>
+      </c>
+      <c r="E147">
+        <v>485452900</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
ArrayList -> int[] for memory save
</commit_message>
<xml_diff>
--- a/Task_2_1_1/time.xlsx
+++ b/Task_2_1_1/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\NSU\OOP\Task_2_1_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C783D4B4-3095-466D-98A8-86322C31BB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE64AC8F-EB5A-4CE8-B07F-BD227DAD8706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D5ABC52E-7C61-45CD-9E16-B81EF21C7B9D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>Usual</t>
   </si>
@@ -57,7 +57,7 @@
     <t>arr.length = 1kk</t>
   </si>
   <si>
-    <t>arr.length = 100k</t>
+    <t>с 10-кратным повторением (поделил на 10 потом)</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,15 +87,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -153,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -167,7 +158,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -284,205 +274,216 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$C$42:$C$72</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+            <c:strRef>
+              <c:f>Лист1!$C$40:$C$72</c:f>
+              <c:strCache>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
+                  <c:v>Usual</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Optimus (Stream)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>31</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$42:$D$72</c:f>
+              <c:f>Лист1!$D$40:$D$72</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>0.36516666666666669</c:v>
+                  <c:v>33.545449999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33176666666666671</c:v>
+                  <c:v>102.09437333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4088</c:v>
+                  <c:v>31.84225</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4234</c:v>
+                  <c:v>286.87023999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4264</c:v>
+                  <c:v>354.46147333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.435</c:v>
+                  <c:v>377.6347566666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43969999999999998</c:v>
+                  <c:v>433.45422333333335</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.55210000000000004</c:v>
+                  <c:v>437.4499633333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.56720000000000004</c:v>
+                  <c:v>410.13909666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.60363333333333336</c:v>
+                  <c:v>403.21022999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.64136666666666664</c:v>
+                  <c:v>422.72969333333327</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.69653333333333345</c:v>
+                  <c:v>408.34453999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.73799999999999999</c:v>
+                  <c:v>382.1543733333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2566666666666668</c:v>
+                  <c:v>373.7577766666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.82023333333333337</c:v>
+                  <c:v>349.93829333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.84033333333333338</c:v>
+                  <c:v>349.15191666666669</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.95563333333333333</c:v>
+                  <c:v>334.30834999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.7404999999999999</c:v>
+                  <c:v>320.80375666666669</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1255666666666668</c:v>
+                  <c:v>330.76777000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.2076333333333331</c:v>
+                  <c:v>329.44851</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4201333333333337</c:v>
+                  <c:v>318.64961999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5143333333333333</c:v>
+                  <c:v>316.99907000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.5115666666666667</c:v>
+                  <c:v>313.93516999999997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.2510999999999999</c:v>
+                  <c:v>326.15464666666668</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.3248333333333333</c:v>
+                  <c:v>317.04913666666664</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.5193666666666668</c:v>
+                  <c:v>322.84330666666671</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.7243666666666668</c:v>
+                  <c:v>362.56063666666665</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.4458666666666669</c:v>
+                  <c:v>327.00149333333331</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.4727666666666666</c:v>
+                  <c:v>318.19207333333333</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.4951333333333332</c:v>
+                  <c:v>328.18165000000005</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.6969333333333332</c:v>
+                  <c:v>360.72090999999995</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>360.95258000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>342.80452000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,103 +1355,103 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>4033.3507999999997</c:v>
+                  <c:v>23.286999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2361.6039999999998</c:v>
+                  <c:v>35.515500000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4093.4922999999999</c:v>
+                  <c:v>17.363849999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2023.3779</c:v>
+                  <c:v>45.317999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4467.8284000000003</c:v>
+                  <c:v>52.698250000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4519.5195999999996</c:v>
+                  <c:v>41.61795</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4636.1889000000001</c:v>
+                  <c:v>43.782249999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4794.2619000000004</c:v>
+                  <c:v>41.986050000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5055.3064999999997</c:v>
+                  <c:v>42.423250000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5118.8723</c:v>
+                  <c:v>43.198250000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5304.3768</c:v>
+                  <c:v>37.142400000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5386.2038000000002</c:v>
+                  <c:v>40.909550000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5461.3427000000001</c:v>
+                  <c:v>36.543550000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5596.9142000000002</c:v>
+                  <c:v>36.555199999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5718.4560000000001</c:v>
+                  <c:v>36.462449999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5848.3908000000001</c:v>
+                  <c:v>34.431650000000005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5888.8244999999997</c:v>
+                  <c:v>33.344149999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5869.1355999999996</c:v>
+                  <c:v>32.16545</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5891.8882000000003</c:v>
+                  <c:v>32.469349999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5939.5755999999992</c:v>
+                  <c:v>33.022150000000003</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5869.9935999999998</c:v>
+                  <c:v>33.774149999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6478.9552999999996</c:v>
+                  <c:v>32.425849999999997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6675.9492</c:v>
+                  <c:v>33.772599999999997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6655.8872999999994</c:v>
+                  <c:v>35.000599999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6223.5045</c:v>
+                  <c:v>34.5334</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5958.7987999999996</c:v>
+                  <c:v>34.182250000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5958.3064999999997</c:v>
+                  <c:v>32.964150000000004</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5965.9070999999994</c:v>
+                  <c:v>35.02225</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5958.8387000000002</c:v>
+                  <c:v>33.097749999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5962.8292999999994</c:v>
+                  <c:v>32.353650000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5986.7290000000003</c:v>
+                  <c:v>33.407849999999996</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5987.3458000000001</c:v>
+                  <c:v>30.833200000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5979.7764999999999</c:v>
+                  <c:v>31.266349999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1633,773 +1634,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ru-RU"/>
-              <a:t>в</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t> милл</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t>исекундах</a:t>
-            </a:r>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Лист1!$C$40:$C$41</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Usual</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Optimus (Stream)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$D$40:$D$41</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>25.169033333333331</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>221.53556666666665</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9C6A-46D4-8FA3-E72E958E7901}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1836500703"/>
-        <c:axId val="1444802431"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1836500703"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1444802431"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1444802431"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1836500703"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Лист1!$C$115:$C$147</c:f>
-              <c:strCache>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>Usual</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Optimus (Stream)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$D$115:$D$147</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>440.57440000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>72.147800000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>407.4178</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>286.54259999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>345.58659999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>364.52300000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>377.18629999999996</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>408.1694</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>415.90679999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>428.93259999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>433.64709999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>454.58190000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>462.5874</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>457.76609999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>467.89690000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>474.00009999999997</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>474.45269999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>476.02719999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>474.46</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>479.73940000000005</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>480.20729999999998</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>476.40209999999996</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>475.77979999999997</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>481.5213</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>479.98990000000003</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>483.58340000000004</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>488.98359999999997</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>485.46290000000005</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>481.93079999999998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>489.17720000000003</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>488.79950000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>489.85950000000003</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>485.4529</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-91B8-447E-A401-C95509E4587F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="2004431967"/>
-        <c:axId val="1886563039"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2004431967"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1886563039"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1886563039"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2004431967"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2520,86 +1754,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3607,1012 +2761,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5220,78 +3368,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>308161</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>11207</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A193F9DF-7C75-47CF-9027-F635E1CDCC90}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>604571</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>423333</xdr:colOff>
-      <xdr:row>147</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Диаграмма 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DEEDB6F-45DA-48A6-8B90-3ECEB270BFD4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5599,18 +3675,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D94D687-82E9-4018-8178-D13A8669E2BA}">
   <dimension ref="B2:AG147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="8" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
@@ -5640,12 +3715,14 @@
       </c>
       <c r="D3" s="10">
         <f>SUM(E3:N3) / COUNT(E3:N3)/ 1000 / 1000</f>
-        <v>4033.3507999999997</v>
+        <v>23.286999999999999</v>
       </c>
       <c r="E3" s="1">
-        <v>4033350800</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>23847200</v>
+      </c>
+      <c r="F3" s="1">
+        <v>22726800</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -5661,12 +3738,14 @@
       </c>
       <c r="D4" s="10">
         <f t="shared" ref="D4:D35" si="0">SUM(E4:N4) / COUNT(E4:N4)/ 1000 / 1000</f>
-        <v>2361.6039999999998</v>
+        <v>35.515500000000003</v>
       </c>
       <c r="E4" s="1">
-        <v>2361604000</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>43068800</v>
+      </c>
+      <c r="F4" s="1">
+        <v>27962200</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -5685,12 +3764,14 @@
       </c>
       <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>4093.4922999999999</v>
+        <v>17.363849999999999</v>
       </c>
       <c r="E5" s="1">
-        <v>4093492300</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>17070500</v>
+      </c>
+      <c r="F5" s="1">
+        <v>17657200</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -5707,12 +3788,14 @@
       </c>
       <c r="D6" s="10">
         <f t="shared" si="0"/>
-        <v>2023.3779</v>
+        <v>45.317999999999998</v>
       </c>
       <c r="E6" s="1">
-        <v>2023377900</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>34034800</v>
+      </c>
+      <c r="F6" s="1">
+        <v>56601200</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -5729,12 +3812,14 @@
       </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
-        <v>4467.8284000000003</v>
+        <v>52.698250000000002</v>
       </c>
       <c r="E7" s="1">
-        <v>4467828400</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>55877500</v>
+      </c>
+      <c r="F7" s="1">
+        <v>49519000</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -5752,12 +3837,14 @@
       </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
-        <v>4519.5195999999996</v>
+        <v>41.61795</v>
       </c>
       <c r="E8" s="1">
-        <v>4519519600</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>38368400</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44867500</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -5775,12 +3862,14 @@
       </c>
       <c r="D9" s="10">
         <f t="shared" si="0"/>
-        <v>4636.1889000000001</v>
+        <v>43.782249999999998</v>
       </c>
       <c r="E9" s="1">
-        <v>4636188900</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>42445500</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45119000</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -5798,12 +3887,14 @@
       </c>
       <c r="D10" s="10">
         <f t="shared" si="0"/>
-        <v>4794.2619000000004</v>
+        <v>41.986050000000006</v>
       </c>
       <c r="E10" s="1">
-        <v>4794261900</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>43871300</v>
+      </c>
+      <c r="F10" s="1">
+        <v>40100800</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -5821,12 +3912,14 @@
       </c>
       <c r="D11" s="10">
         <f t="shared" si="0"/>
-        <v>5055.3064999999997</v>
+        <v>42.423250000000003</v>
       </c>
       <c r="E11" s="1">
-        <v>5055306500</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>41498800</v>
+      </c>
+      <c r="F11" s="1">
+        <v>43347700</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -5844,12 +3937,14 @@
       </c>
       <c r="D12" s="10">
         <f t="shared" si="0"/>
-        <v>5118.8723</v>
+        <v>43.198250000000002</v>
       </c>
       <c r="E12" s="1">
-        <v>5118872300</v>
-      </c>
-      <c r="F12" s="1"/>
+        <v>42146400</v>
+      </c>
+      <c r="F12" s="1">
+        <v>44250100</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -5867,12 +3962,14 @@
       </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>5304.3768</v>
+        <v>37.142400000000002</v>
       </c>
       <c r="E13" s="1">
-        <v>5304376800</v>
-      </c>
-      <c r="F13" s="1"/>
+        <v>38486800</v>
+      </c>
+      <c r="F13" s="1">
+        <v>35798000</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -5890,12 +3987,14 @@
       </c>
       <c r="D14" s="10">
         <f t="shared" si="0"/>
-        <v>5386.2038000000002</v>
+        <v>40.909550000000003</v>
       </c>
       <c r="E14" s="1">
-        <v>5386203800</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>43308400</v>
+      </c>
+      <c r="F14" s="1">
+        <v>38510700</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -5913,12 +4012,14 @@
       </c>
       <c r="D15" s="10">
         <f t="shared" si="0"/>
-        <v>5461.3427000000001</v>
+        <v>36.543550000000003</v>
       </c>
       <c r="E15" s="1">
-        <v>5461342700</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>40023400</v>
+      </c>
+      <c r="F15" s="1">
+        <v>33063700</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -5936,12 +4037,14 @@
       </c>
       <c r="D16" s="10">
         <f t="shared" si="0"/>
-        <v>5596.9142000000002</v>
+        <v>36.555199999999999</v>
       </c>
       <c r="E16" s="1">
-        <v>5596914200</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>37513500</v>
+      </c>
+      <c r="F16" s="1">
+        <v>35596900</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -5959,12 +4062,14 @@
       </c>
       <c r="D17" s="10">
         <f t="shared" si="0"/>
-        <v>5718.4560000000001</v>
+        <v>36.462449999999997</v>
       </c>
       <c r="E17" s="1">
-        <v>5718456000</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>36667300</v>
+      </c>
+      <c r="F17" s="1">
+        <v>36257600</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -5982,12 +4087,14 @@
       </c>
       <c r="D18" s="10">
         <f t="shared" si="0"/>
-        <v>5848.3908000000001</v>
+        <v>34.431650000000005</v>
       </c>
       <c r="E18" s="1">
-        <v>5848390800</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>32566000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>36297300</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -6005,12 +4112,14 @@
       </c>
       <c r="D19" s="10">
         <f t="shared" si="0"/>
-        <v>5888.8244999999997</v>
+        <v>33.344149999999999</v>
       </c>
       <c r="E19" s="1">
-        <v>5888824500</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>30773800</v>
+      </c>
+      <c r="F19" s="1">
+        <v>35914500</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -6028,12 +4137,14 @@
       </c>
       <c r="D20" s="10">
         <f t="shared" si="0"/>
-        <v>5869.1355999999996</v>
+        <v>32.16545</v>
       </c>
       <c r="E20" s="1">
-        <v>5869135600</v>
-      </c>
-      <c r="F20" s="1"/>
+        <v>31039200</v>
+      </c>
+      <c r="F20" s="1">
+        <v>33291700</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -6051,12 +4162,14 @@
       </c>
       <c r="D21" s="10">
         <f t="shared" si="0"/>
-        <v>5891.8882000000003</v>
+        <v>32.469349999999999</v>
       </c>
       <c r="E21" s="1">
-        <v>5891888200</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>30610500</v>
+      </c>
+      <c r="F21" s="1">
+        <v>34328200</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -6074,12 +4187,14 @@
       </c>
       <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>5939.5755999999992</v>
+        <v>33.022150000000003</v>
       </c>
       <c r="E22" s="1">
-        <v>5939575600</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>31587900</v>
+      </c>
+      <c r="F22" s="1">
+        <v>34456400</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -6097,12 +4212,14 @@
       </c>
       <c r="D23" s="10">
         <f t="shared" si="0"/>
-        <v>5869.9935999999998</v>
+        <v>33.774149999999999</v>
       </c>
       <c r="E23" s="1">
-        <v>5869993600</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>32468900</v>
+      </c>
+      <c r="F23" s="1">
+        <v>35079400</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -6120,12 +4237,14 @@
       </c>
       <c r="D24" s="10">
         <f t="shared" si="0"/>
-        <v>6478.9552999999996</v>
+        <v>32.425849999999997</v>
       </c>
       <c r="E24" s="1">
-        <v>6478955300</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>32034500</v>
+      </c>
+      <c r="F24" s="1">
+        <v>32817200</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -6143,12 +4262,14 @@
       </c>
       <c r="D25" s="10">
         <f t="shared" si="0"/>
-        <v>6675.9492</v>
+        <v>33.772599999999997</v>
       </c>
       <c r="E25" s="1">
-        <v>6675949200</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>33594600</v>
+      </c>
+      <c r="F25" s="1">
+        <v>33950600</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -6166,12 +4287,14 @@
       </c>
       <c r="D26" s="10">
         <f t="shared" si="0"/>
-        <v>6655.8872999999994</v>
+        <v>35.000599999999999</v>
       </c>
       <c r="E26" s="1">
-        <v>6655887300</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>33151000</v>
+      </c>
+      <c r="F26" s="1">
+        <v>36850200</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -6189,12 +4312,14 @@
       </c>
       <c r="D27" s="10">
         <f t="shared" si="0"/>
-        <v>6223.5045</v>
+        <v>34.5334</v>
       </c>
       <c r="E27" s="1">
-        <v>6223504500</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>31464400</v>
+      </c>
+      <c r="F27" s="1">
+        <v>37602400</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -6212,12 +4337,14 @@
       </c>
       <c r="D28" s="10">
         <f t="shared" si="0"/>
-        <v>5958.7987999999996</v>
+        <v>34.182250000000003</v>
       </c>
       <c r="E28" s="1">
-        <v>5958798800</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>31338000</v>
+      </c>
+      <c r="F28" s="1">
+        <v>37026500</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -6235,12 +4362,14 @@
       </c>
       <c r="D29" s="10">
         <f t="shared" si="0"/>
-        <v>5958.3064999999997</v>
+        <v>32.964150000000004</v>
       </c>
       <c r="E29" s="1">
-        <v>5958306500</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>33178300</v>
+      </c>
+      <c r="F29" s="1">
+        <v>32750000</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -6258,12 +4387,14 @@
       </c>
       <c r="D30" s="10">
         <f t="shared" si="0"/>
-        <v>5965.9070999999994</v>
+        <v>35.02225</v>
       </c>
       <c r="E30" s="1">
-        <v>5965907100</v>
-      </c>
-      <c r="F30" s="1"/>
+        <v>33487600</v>
+      </c>
+      <c r="F30" s="1">
+        <v>36556900</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -6281,12 +4412,14 @@
       </c>
       <c r="D31" s="10">
         <f t="shared" si="0"/>
-        <v>5958.8387000000002</v>
+        <v>33.097749999999998</v>
       </c>
       <c r="E31" s="1">
-        <v>5958838700</v>
-      </c>
-      <c r="F31" s="1"/>
+        <v>30722200</v>
+      </c>
+      <c r="F31" s="1">
+        <v>35473300</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -6304,12 +4437,14 @@
       </c>
       <c r="D32" s="10">
         <f t="shared" si="0"/>
-        <v>5962.8292999999994</v>
+        <v>32.353650000000002</v>
       </c>
       <c r="E32" s="1">
-        <v>5962829300</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>30693000</v>
+      </c>
+      <c r="F32" s="1">
+        <v>34014300</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -6327,12 +4462,14 @@
       </c>
       <c r="D33" s="10">
         <f t="shared" si="0"/>
-        <v>5986.7290000000003</v>
+        <v>33.407849999999996</v>
       </c>
       <c r="E33" s="1">
-        <v>5986729000</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>32195000</v>
+      </c>
+      <c r="F33" s="1">
+        <v>34620700</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -6350,12 +4487,14 @@
       </c>
       <c r="D34" s="10">
         <f t="shared" si="0"/>
-        <v>5987.3458000000001</v>
+        <v>30.833200000000001</v>
       </c>
       <c r="E34" s="1">
-        <v>5987345800</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>30919500</v>
+      </c>
+      <c r="F34" s="1">
+        <v>30746900</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -6373,12 +4512,14 @@
       </c>
       <c r="D35" s="10">
         <f t="shared" si="0"/>
-        <v>5979.7764999999999</v>
+        <v>31.266349999999999</v>
       </c>
       <c r="E35" s="1">
-        <v>5979776500</v>
-      </c>
-      <c r="F35" s="1"/>
+        <v>30731800</v>
+      </c>
+      <c r="F35" s="1">
+        <v>31800900</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -6415,26 +4556,27 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="40" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>1</v>
-      </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="5">
-        <f>SUM(E40:N40) / COUNT(E40:N40)/ 1000 / 1000 / B40</f>
-        <v>25.169033333333331</v>
+        <f>SUM(E40:N40) / COUNT(E40:N40)/ 1000 / 1000</f>
+        <v>33.545449999999995</v>
       </c>
       <c r="E40" s="1">
-        <v>25651700</v>
-      </c>
-      <c r="F40" s="13">
-        <v>24927700</v>
+        <v>28433300</v>
+      </c>
+      <c r="F40" s="1">
+        <v>47469700</v>
       </c>
       <c r="G40" s="1">
-        <v>24927700</v>
+        <f>AG40/10</f>
+        <v>24733350</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -6448,24 +4590,22 @@
       </c>
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>1</v>
-      </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="5">
-        <f>SUM(E41:N41) / COUNT(E41:N41)/ 1000 / 1000 / B41</f>
-        <v>221.53556666666665</v>
+        <f t="shared" ref="D41:D72" si="1">SUM(E41:N41) / COUNT(E41:N41)/ 1000 / 1000</f>
+        <v>102.09437333333332</v>
       </c>
       <c r="E41" s="1">
-        <v>219793300</v>
+        <v>49979400</v>
       </c>
       <c r="F41" s="1">
-        <v>222406700</v>
+        <v>52847000</v>
       </c>
       <c r="G41" s="1">
-        <v>222406700</v>
+        <f t="shared" ref="G41:G72" si="2">AG41/10</f>
+        <v>203456720</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -6486,17 +4626,18 @@
         <v>1</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" ref="D42:D72" si="1">SUM(E42:N42) / COUNT(E42:N42)/ 1000 / 1000</f>
-        <v>0.36516666666666669</v>
+        <f t="shared" si="1"/>
+        <v>31.84225</v>
       </c>
       <c r="E42" s="1">
-        <v>334300</v>
+        <v>32539000</v>
       </c>
       <c r="F42" s="1">
-        <v>380600</v>
+        <v>39680700</v>
       </c>
       <c r="G42" s="1">
-        <v>380600</v>
+        <f t="shared" si="2"/>
+        <v>23307050</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -6516,16 +4657,17 @@
       </c>
       <c r="D43" s="5">
         <f t="shared" si="1"/>
-        <v>0.33176666666666671</v>
+        <v>286.87023999999997</v>
       </c>
       <c r="E43" s="1">
-        <v>345300</v>
+        <v>244041400</v>
       </c>
       <c r="F43" s="1">
-        <v>325000</v>
+        <v>300531500</v>
       </c>
       <c r="G43" s="1">
-        <v>325000</v>
+        <f t="shared" si="2"/>
+        <v>316037820</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -6545,16 +4687,17 @@
       </c>
       <c r="D44" s="5">
         <f t="shared" si="1"/>
-        <v>0.4088</v>
+        <v>354.46147333333334</v>
       </c>
       <c r="E44" s="1">
-        <v>343600</v>
+        <v>357423100</v>
       </c>
       <c r="F44" s="1">
-        <v>441400</v>
+        <v>331776400</v>
       </c>
       <c r="G44" s="1">
-        <v>441400</v>
+        <f t="shared" si="2"/>
+        <v>374184920</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -6574,16 +4717,17 @@
       </c>
       <c r="D45" s="5">
         <f t="shared" si="1"/>
-        <v>0.4234</v>
+        <v>377.6347566666667</v>
       </c>
       <c r="E45" s="1">
-        <v>404600</v>
+        <v>345213600</v>
       </c>
       <c r="F45" s="1">
-        <v>432800</v>
+        <v>361984100</v>
       </c>
       <c r="G45" s="1">
-        <v>432800</v>
+        <f t="shared" si="2"/>
+        <v>425706570</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -6603,16 +4747,17 @@
       </c>
       <c r="D46" s="5">
         <f t="shared" si="1"/>
-        <v>0.4264</v>
+        <v>433.45422333333335</v>
       </c>
       <c r="E46" s="1">
-        <v>350200</v>
+        <v>409804400</v>
       </c>
       <c r="F46" s="1">
-        <v>464500</v>
+        <v>400214900</v>
       </c>
       <c r="G46" s="1">
-        <v>464500</v>
+        <f t="shared" si="2"/>
+        <v>490343370</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -6632,16 +4777,17 @@
       </c>
       <c r="D47" s="5">
         <f t="shared" si="1"/>
-        <v>0.435</v>
+        <v>437.4499633333333</v>
       </c>
       <c r="E47" s="1">
-        <v>502600</v>
+        <v>430005300</v>
       </c>
       <c r="F47" s="1">
-        <v>401200</v>
+        <v>397526700</v>
       </c>
       <c r="G47" s="1">
-        <v>401200</v>
+        <f t="shared" si="2"/>
+        <v>484817890</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -6661,16 +4807,17 @@
       </c>
       <c r="D48" s="5">
         <f t="shared" si="1"/>
-        <v>0.43969999999999998</v>
+        <v>410.13909666666666</v>
       </c>
       <c r="E48" s="1">
-        <v>430900</v>
+        <v>361169300</v>
       </c>
       <c r="F48" s="1">
-        <v>444100</v>
+        <v>396955300</v>
       </c>
       <c r="G48" s="1">
-        <v>444100</v>
+        <f t="shared" si="2"/>
+        <v>472292690</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -6690,16 +4837,17 @@
       </c>
       <c r="D49" s="5">
         <f t="shared" si="1"/>
-        <v>0.55210000000000004</v>
+        <v>403.21022999999997</v>
       </c>
       <c r="E49" s="1">
-        <v>581700</v>
+        <v>356284800</v>
       </c>
       <c r="F49" s="1">
-        <v>537300</v>
+        <v>369938800</v>
       </c>
       <c r="G49" s="1">
-        <v>537300</v>
+        <f t="shared" si="2"/>
+        <v>483407090</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -6719,16 +4867,17 @@
       </c>
       <c r="D50" s="5">
         <f t="shared" si="1"/>
-        <v>0.56720000000000004</v>
+        <v>422.72969333333327</v>
       </c>
       <c r="E50" s="1">
-        <v>582600</v>
+        <v>373302800</v>
       </c>
       <c r="F50" s="1">
-        <v>559500</v>
+        <v>394570600</v>
       </c>
       <c r="G50" s="1">
-        <v>559500</v>
+        <f t="shared" si="2"/>
+        <v>500315680</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -6748,16 +4897,17 @@
       </c>
       <c r="D51" s="5">
         <f t="shared" si="1"/>
-        <v>0.60363333333333336</v>
+        <v>408.34453999999999</v>
       </c>
       <c r="E51" s="1">
-        <v>622300</v>
+        <v>366315400</v>
       </c>
       <c r="F51" s="1">
-        <v>594300</v>
+        <v>368913500</v>
       </c>
       <c r="G51" s="1">
-        <v>594300</v>
+        <f t="shared" si="2"/>
+        <v>489804720</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -6777,16 +4927,17 @@
       </c>
       <c r="D52" s="5">
         <f t="shared" si="1"/>
-        <v>0.64136666666666664</v>
+        <v>382.1543733333333</v>
       </c>
       <c r="E52" s="1">
-        <v>683100</v>
+        <v>328730900</v>
       </c>
       <c r="F52" s="1">
-        <v>620500</v>
+        <v>362363700</v>
       </c>
       <c r="G52" s="1">
-        <v>620500</v>
+        <f t="shared" si="2"/>
+        <v>455368520</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -6806,16 +4957,17 @@
       </c>
       <c r="D53" s="5">
         <f t="shared" si="1"/>
-        <v>0.69653333333333345</v>
+        <v>373.7577766666667</v>
       </c>
       <c r="E53" s="1">
-        <v>719000</v>
+        <v>332586300</v>
       </c>
       <c r="F53" s="1">
-        <v>685300</v>
+        <v>350982800</v>
       </c>
       <c r="G53" s="1">
-        <v>685300</v>
+        <f t="shared" si="2"/>
+        <v>437704230</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -6835,16 +4987,17 @@
       </c>
       <c r="D54" s="5">
         <f t="shared" si="1"/>
-        <v>0.73799999999999999</v>
+        <v>349.93829333333332</v>
       </c>
       <c r="E54" s="1">
-        <v>753400</v>
+        <v>316142600</v>
       </c>
       <c r="F54" s="1">
-        <v>730300</v>
+        <v>332955200</v>
       </c>
       <c r="G54" s="1">
-        <v>730300</v>
+        <f t="shared" si="2"/>
+        <v>400717080</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -6864,16 +5017,17 @@
       </c>
       <c r="D55" s="5">
         <f t="shared" si="1"/>
-        <v>1.2566666666666668</v>
+        <v>349.15191666666669</v>
       </c>
       <c r="E55" s="1">
-        <v>830800</v>
+        <v>329674800</v>
       </c>
       <c r="F55" s="1">
-        <v>1469600</v>
+        <v>330660700</v>
       </c>
       <c r="G55" s="1">
-        <v>1469600</v>
+        <f t="shared" si="2"/>
+        <v>387120250</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -6893,16 +5047,17 @@
       </c>
       <c r="D56" s="5">
         <f t="shared" si="1"/>
-        <v>0.82023333333333337</v>
+        <v>334.30834999999996</v>
       </c>
       <c r="E56" s="1">
-        <v>791900</v>
+        <v>311630700</v>
       </c>
       <c r="F56" s="1">
-        <v>834400</v>
+        <v>319788100</v>
       </c>
       <c r="G56" s="1">
-        <v>834400</v>
+        <f t="shared" si="2"/>
+        <v>371506250</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -6922,16 +5077,17 @@
       </c>
       <c r="D57" s="5">
         <f t="shared" si="1"/>
-        <v>0.84033333333333338</v>
+        <v>320.80375666666669</v>
       </c>
       <c r="E57" s="1">
-        <v>864200</v>
+        <v>304338000</v>
       </c>
       <c r="F57" s="1">
-        <v>828400</v>
+        <v>305499100</v>
       </c>
       <c r="G57" s="1">
-        <v>828400</v>
+        <f t="shared" si="2"/>
+        <v>352574170</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -6951,16 +5107,17 @@
       </c>
       <c r="D58" s="5">
         <f t="shared" si="1"/>
-        <v>0.95563333333333333</v>
+        <v>330.76777000000004</v>
       </c>
       <c r="E58" s="1">
-        <v>973300</v>
+        <v>316924000</v>
       </c>
       <c r="F58" s="1">
-        <v>946800</v>
+        <v>310097300</v>
       </c>
       <c r="G58" s="1">
-        <v>946800</v>
+        <f t="shared" si="2"/>
+        <v>365282010</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -6980,16 +5137,17 @@
       </c>
       <c r="D59" s="5">
         <f t="shared" si="1"/>
-        <v>1.7404999999999999</v>
+        <v>329.44851</v>
       </c>
       <c r="E59" s="1">
-        <v>1177300</v>
+        <v>300466100</v>
       </c>
       <c r="F59" s="1">
-        <v>2022100</v>
+        <v>312368400</v>
       </c>
       <c r="G59" s="1">
-        <v>2022100</v>
+        <f t="shared" si="2"/>
+        <v>375511030</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -7009,16 +5167,17 @@
       </c>
       <c r="D60" s="5">
         <f t="shared" si="1"/>
-        <v>2.1255666666666668</v>
+        <v>318.64961999999997</v>
       </c>
       <c r="E60" s="1">
-        <v>1059500</v>
+        <v>303160700</v>
       </c>
       <c r="F60" s="1">
-        <v>2658600</v>
+        <v>301508200</v>
       </c>
       <c r="G60" s="1">
-        <v>2658600</v>
+        <f t="shared" si="2"/>
+        <v>351279960</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -7038,16 +5197,17 @@
       </c>
       <c r="D61" s="5">
         <f t="shared" si="1"/>
-        <v>1.2076333333333331</v>
+        <v>316.99907000000002</v>
       </c>
       <c r="E61" s="1">
-        <v>1070900</v>
+        <v>297279900</v>
       </c>
       <c r="F61" s="1">
-        <v>1276000</v>
+        <v>296456600</v>
       </c>
       <c r="G61" s="1">
-        <v>1276000</v>
+        <f t="shared" si="2"/>
+        <v>357260710</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -7067,16 +5227,17 @@
       </c>
       <c r="D62" s="5">
         <f t="shared" si="1"/>
-        <v>2.4201333333333337</v>
+        <v>313.93516999999997</v>
       </c>
       <c r="E62" s="1">
-        <v>1390200</v>
+        <v>304024900</v>
       </c>
       <c r="F62" s="1">
-        <v>2935100</v>
+        <v>297238300</v>
       </c>
       <c r="G62" s="1">
-        <v>2935100</v>
+        <f t="shared" si="2"/>
+        <v>340542310</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -7096,16 +5257,17 @@
       </c>
       <c r="D63" s="5">
         <f t="shared" si="1"/>
-        <v>1.5143333333333333</v>
+        <v>326.15464666666668</v>
       </c>
       <c r="E63" s="1">
-        <v>1280400</v>
+        <v>302677200</v>
       </c>
       <c r="F63" s="1">
-        <v>1631300</v>
+        <v>312758700</v>
       </c>
       <c r="G63" s="1">
-        <v>1631300</v>
+        <f t="shared" si="2"/>
+        <v>363028040</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -7125,16 +5287,17 @@
       </c>
       <c r="D64" s="5">
         <f t="shared" si="1"/>
-        <v>1.5115666666666667</v>
+        <v>317.04913666666664</v>
       </c>
       <c r="E64" s="1">
-        <v>1389500</v>
+        <v>297965800</v>
       </c>
       <c r="F64" s="1">
-        <v>1572600</v>
+        <v>303472000</v>
       </c>
       <c r="G64" s="1">
-        <v>1572600</v>
+        <f t="shared" si="2"/>
+        <v>349709610</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -7154,16 +5317,17 @@
       </c>
       <c r="D65" s="5">
         <f t="shared" si="1"/>
-        <v>1.2510999999999999</v>
+        <v>322.84330666666671</v>
       </c>
       <c r="E65" s="1">
-        <v>1167500</v>
+        <v>309177100</v>
       </c>
       <c r="F65" s="1">
-        <v>1292900</v>
+        <v>313048000</v>
       </c>
       <c r="G65" s="1">
-        <v>1292900</v>
+        <f t="shared" si="2"/>
+        <v>346304820</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -7183,16 +5347,17 @@
       </c>
       <c r="D66" s="5">
         <f t="shared" si="1"/>
-        <v>1.3248333333333333</v>
+        <v>362.56063666666665</v>
       </c>
       <c r="E66" s="1">
-        <v>1325300</v>
+        <v>303775000</v>
       </c>
       <c r="F66" s="1">
-        <v>1324600</v>
+        <v>431818300</v>
       </c>
       <c r="G66" s="1">
-        <v>1324600</v>
+        <f t="shared" si="2"/>
+        <v>352088610</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -7212,16 +5377,17 @@
       </c>
       <c r="D67" s="5">
         <f t="shared" si="1"/>
-        <v>1.5193666666666668</v>
+        <v>327.00149333333331</v>
       </c>
       <c r="E67" s="1">
-        <v>1592100</v>
+        <v>313496500</v>
       </c>
       <c r="F67" s="1">
-        <v>1483000</v>
+        <v>322596400</v>
       </c>
       <c r="G67" s="1">
-        <v>1483000</v>
+        <f t="shared" si="2"/>
+        <v>344911580</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -7241,16 +5407,17 @@
       </c>
       <c r="D68" s="5">
         <f t="shared" si="1"/>
-        <v>1.7243666666666668</v>
+        <v>318.19207333333333</v>
       </c>
       <c r="E68" s="1">
-        <v>2038100</v>
+        <v>299808300</v>
       </c>
       <c r="F68" s="1">
-        <v>1567500</v>
+        <v>306056000</v>
       </c>
       <c r="G68" s="1">
-        <v>1567500</v>
+        <f t="shared" si="2"/>
+        <v>348711920</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -7270,16 +5437,17 @@
       </c>
       <c r="D69" s="5">
         <f t="shared" si="1"/>
-        <v>1.4458666666666669</v>
+        <v>328.18165000000005</v>
       </c>
       <c r="E69" s="1">
-        <v>1583600</v>
+        <v>313287100</v>
       </c>
       <c r="F69" s="1">
-        <v>1377000</v>
+        <v>326549700</v>
       </c>
       <c r="G69" s="1">
-        <v>1377000</v>
+        <f t="shared" si="2"/>
+        <v>344708150</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
@@ -7299,16 +5467,17 @@
       </c>
       <c r="D70" s="5">
         <f t="shared" si="1"/>
-        <v>1.4727666666666666</v>
+        <v>360.72090999999995</v>
       </c>
       <c r="E70" s="1">
-        <v>1738500</v>
+        <v>304203800</v>
       </c>
       <c r="F70" s="1">
-        <v>1339900</v>
+        <v>426975400</v>
       </c>
       <c r="G70" s="1">
-        <v>1339900</v>
+        <f t="shared" si="2"/>
+        <v>350983530</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
@@ -7328,16 +5497,17 @@
       </c>
       <c r="D71" s="5">
         <f t="shared" si="1"/>
-        <v>1.4951333333333332</v>
+        <v>360.95258000000001</v>
       </c>
       <c r="E71" s="1">
-        <v>1692600</v>
+        <v>306587100</v>
       </c>
       <c r="F71" s="1">
-        <v>1396400</v>
+        <v>417802500</v>
       </c>
       <c r="G71" s="1">
-        <v>1396400</v>
+        <f t="shared" si="2"/>
+        <v>358468140</v>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
@@ -7357,16 +5527,17 @@
       </c>
       <c r="D72" s="5">
         <f t="shared" si="1"/>
-        <v>1.6969333333333332</v>
+        <v>342.80452000000002</v>
       </c>
       <c r="E72" s="1">
-        <v>1838800</v>
+        <v>304619800</v>
       </c>
       <c r="F72" s="1">
-        <v>1626000</v>
+        <v>364964000</v>
       </c>
       <c r="G72" s="1">
-        <v>1626000</v>
+        <f t="shared" si="2"/>
+        <v>358829760</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
@@ -7436,7 +5607,7 @@
         <v>2</v>
       </c>
       <c r="D78" s="5">
-        <f t="shared" ref="D78:D109" si="2">SUM(E78:N78) / COUNT(E78:N78)/ 1000 / 1000</f>
+        <f t="shared" ref="D78:D109" si="3">SUM(E78:N78) / COUNT(E78:N78)/ 1000 / 1000</f>
         <v>968.4126</v>
       </c>
       <c r="E78" s="1">
@@ -7466,7 +5637,7 @@
         <v>1</v>
       </c>
       <c r="D79" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>220.41729999999998</v>
       </c>
       <c r="E79" s="1">
@@ -7494,7 +5665,7 @@
         <v>2</v>
       </c>
       <c r="D80" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2520.1049750000002</v>
       </c>
       <c r="E80" s="1">
@@ -7522,7 +5693,7 @@
         <v>3</v>
       </c>
       <c r="D81" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3125.7725</v>
       </c>
       <c r="E81" s="1">
@@ -7550,7 +5721,7 @@
         <v>4</v>
       </c>
       <c r="D82" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3732.9300750000002</v>
       </c>
       <c r="E82" s="1">
@@ -7578,7 +5749,7 @@
         <v>5</v>
       </c>
       <c r="D83" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3659.3316500000001</v>
       </c>
       <c r="E83" s="1">
@@ -7606,7 +5777,7 @@
         <v>6</v>
       </c>
       <c r="D84" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3422.7775499999998</v>
       </c>
       <c r="E84" s="1">
@@ -7634,7 +5805,7 @@
         <v>7</v>
       </c>
       <c r="D85" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3099.3313750000002</v>
       </c>
       <c r="E85" s="1">
@@ -7662,7 +5833,7 @@
         <v>8</v>
       </c>
       <c r="D86" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3121.9437749999997</v>
       </c>
       <c r="E86" s="1">
@@ -7690,7 +5861,7 @@
         <v>9</v>
       </c>
       <c r="D87" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3171.8808749999998</v>
       </c>
       <c r="E87" s="1">
@@ -7718,7 +5889,7 @@
         <v>10</v>
       </c>
       <c r="D88" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3155.7731749999998</v>
       </c>
       <c r="E88" s="1">
@@ -7746,7 +5917,7 @@
         <v>11</v>
       </c>
       <c r="D89" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3163.0625249999998</v>
       </c>
       <c r="E89" s="1">
@@ -7774,7 +5945,7 @@
         <v>12</v>
       </c>
       <c r="D90" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3258.3580499999998</v>
       </c>
       <c r="E90" s="1">
@@ -7802,7 +5973,7 @@
         <v>13</v>
       </c>
       <c r="D91" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3264.6103499999999</v>
       </c>
       <c r="E91" s="1">
@@ -7830,7 +6001,7 @@
         <v>14</v>
       </c>
       <c r="D92" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3187.1091499999998</v>
       </c>
       <c r="E92" s="1">
@@ -7858,7 +6029,7 @@
         <v>15</v>
       </c>
       <c r="D93" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3352.389525</v>
       </c>
       <c r="E93" s="1">
@@ -7886,7 +6057,7 @@
         <v>16</v>
       </c>
       <c r="D94" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3198.14455</v>
       </c>
       <c r="E94" s="1">
@@ -7914,7 +6085,7 @@
         <v>17</v>
       </c>
       <c r="D95" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3168.8187749999997</v>
       </c>
       <c r="E95" s="1">
@@ -7942,7 +6113,7 @@
         <v>18</v>
       </c>
       <c r="D96" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3163.9285249999998</v>
       </c>
       <c r="E96" s="1">
@@ -7970,7 +6141,7 @@
         <v>19</v>
       </c>
       <c r="D97" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3142.725375</v>
       </c>
       <c r="E97" s="1">
@@ -7998,7 +6169,7 @@
         <v>20</v>
       </c>
       <c r="D98" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3241.3328999999999</v>
       </c>
       <c r="E98" s="1">
@@ -8026,7 +6197,7 @@
         <v>21</v>
       </c>
       <c r="D99" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3198.67355</v>
       </c>
       <c r="E99" s="1">
@@ -8054,7 +6225,7 @@
         <v>22</v>
       </c>
       <c r="D100" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3290.8587000000002</v>
       </c>
       <c r="E100" s="1">
@@ -8082,7 +6253,7 @@
         <v>23</v>
       </c>
       <c r="D101" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3143.5763999999999</v>
       </c>
       <c r="E101" s="1">
@@ -8110,7 +6281,7 @@
         <v>24</v>
       </c>
       <c r="D102" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2768.4515499999998</v>
       </c>
       <c r="E102" s="1">
@@ -8138,7 +6309,7 @@
         <v>25</v>
       </c>
       <c r="D103" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2509.0195750000003</v>
       </c>
       <c r="E103" s="1">
@@ -8166,7 +6337,7 @@
         <v>26</v>
       </c>
       <c r="D104" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2572.3301749999996</v>
       </c>
       <c r="E104" s="1">
@@ -8194,7 +6365,7 @@
         <v>27</v>
       </c>
       <c r="D105" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2580.5604500000004</v>
       </c>
       <c r="E105" s="1">
@@ -8222,7 +6393,7 @@
         <v>28</v>
       </c>
       <c r="D106" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2763.2431499999998</v>
       </c>
       <c r="E106" s="1">
@@ -8250,7 +6421,7 @@
         <v>29</v>
       </c>
       <c r="D107" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3042.1008500000003</v>
       </c>
       <c r="E107" s="1">
@@ -8278,7 +6449,7 @@
         <v>30</v>
       </c>
       <c r="D108" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3287.0614500000001</v>
       </c>
       <c r="E108" s="1">
@@ -8306,7 +6477,7 @@
         <v>31</v>
       </c>
       <c r="D109" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3291.7092000000002</v>
       </c>
       <c r="E109" s="1">
@@ -8328,445 +6499,98 @@
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C115" t="s">
-        <v>0</v>
-      </c>
-      <c r="D115" s="5">
-        <f>SUM(E115:N115) / COUNT(E115:N115)/ 1000 / 1000</f>
-        <v>440.57440000000003</v>
-      </c>
-      <c r="E115">
-        <v>440574400</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C116" t="s">
-        <v>2</v>
-      </c>
-      <c r="D116" s="5">
-        <f t="shared" ref="D116:D147" si="3">SUM(E116:N116) / COUNT(E116:N116)/ 1000 / 1000</f>
-        <v>72.147800000000004</v>
-      </c>
-      <c r="E116">
-        <v>72147800</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C117" s="7">
-        <v>1</v>
-      </c>
-      <c r="D117" s="5">
-        <f t="shared" si="3"/>
-        <v>407.4178</v>
-      </c>
-      <c r="E117">
-        <v>407417800</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="6"/>
-      <c r="C118" s="7">
-        <v>2</v>
-      </c>
-      <c r="D118" s="5">
-        <f t="shared" si="3"/>
-        <v>286.54259999999999</v>
-      </c>
-      <c r="E118">
-        <v>286542600</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="6"/>
-      <c r="C119" s="7">
-        <v>3</v>
-      </c>
-      <c r="D119" s="5">
-        <f t="shared" si="3"/>
-        <v>345.58659999999998</v>
-      </c>
-      <c r="E119">
-        <v>345586600</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B120" s="6"/>
-      <c r="C120" s="7">
-        <v>4</v>
-      </c>
-      <c r="D120" s="5">
-        <f t="shared" si="3"/>
-        <v>364.52300000000002</v>
-      </c>
-      <c r="E120">
-        <v>364523000</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B121" s="6"/>
-      <c r="C121" s="7">
-        <v>5</v>
-      </c>
-      <c r="D121" s="5">
-        <f t="shared" si="3"/>
-        <v>377.18629999999996</v>
-      </c>
-      <c r="E121">
-        <v>377186300</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="6"/>
-      <c r="C122" s="7">
-        <v>6</v>
-      </c>
-      <c r="D122" s="5">
-        <f t="shared" si="3"/>
-        <v>408.1694</v>
-      </c>
-      <c r="E122">
-        <v>408169400</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B123" s="6"/>
-      <c r="C123" s="7">
-        <v>7</v>
-      </c>
-      <c r="D123" s="5">
-        <f t="shared" si="3"/>
-        <v>415.90679999999998</v>
-      </c>
-      <c r="E123">
-        <v>415906800</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B124" s="6"/>
-      <c r="C124" s="7">
-        <v>8</v>
-      </c>
-      <c r="D124" s="5">
-        <f t="shared" si="3"/>
-        <v>428.93259999999998</v>
-      </c>
-      <c r="E124">
-        <v>428932600</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="6"/>
-      <c r="C125" s="7">
-        <v>9</v>
-      </c>
-      <c r="D125" s="5">
-        <f t="shared" si="3"/>
-        <v>433.64709999999997</v>
-      </c>
-      <c r="E125">
-        <v>433647100</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B126" s="6"/>
-      <c r="C126" s="7">
-        <v>10</v>
-      </c>
-      <c r="D126" s="5">
-        <f t="shared" si="3"/>
-        <v>454.58190000000002</v>
-      </c>
-      <c r="E126">
-        <v>454581900</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="6"/>
-      <c r="C127" s="7">
-        <v>11</v>
-      </c>
-      <c r="D127" s="5">
-        <f t="shared" si="3"/>
-        <v>462.5874</v>
-      </c>
-      <c r="E127">
-        <v>462587400</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="6"/>
-      <c r="C128" s="7">
-        <v>12</v>
-      </c>
-      <c r="D128" s="5">
-        <f t="shared" si="3"/>
-        <v>457.76609999999999</v>
-      </c>
-      <c r="E128">
-        <v>457766100</v>
-      </c>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B129" s="6"/>
-      <c r="C129" s="7">
-        <v>13</v>
-      </c>
-      <c r="D129" s="5">
-        <f t="shared" si="3"/>
-        <v>467.89690000000002</v>
-      </c>
-      <c r="E129">
-        <v>467896900</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B130" s="6"/>
-      <c r="C130" s="7">
-        <v>14</v>
-      </c>
-      <c r="D130" s="5">
-        <f t="shared" si="3"/>
-        <v>474.00009999999997</v>
-      </c>
-      <c r="E130">
-        <v>474000100</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B131" s="6"/>
-      <c r="C131" s="7">
-        <v>15</v>
-      </c>
-      <c r="D131" s="5">
-        <f t="shared" si="3"/>
-        <v>474.45269999999999</v>
-      </c>
-      <c r="E131">
-        <v>474452700</v>
-      </c>
-    </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="6"/>
-      <c r="C132" s="7">
-        <v>16</v>
-      </c>
-      <c r="D132" s="5">
-        <f t="shared" si="3"/>
-        <v>476.02719999999999</v>
-      </c>
-      <c r="E132">
-        <v>476027200</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="6"/>
-      <c r="C133" s="7">
-        <v>17</v>
-      </c>
-      <c r="D133" s="5">
-        <f t="shared" si="3"/>
-        <v>474.46</v>
-      </c>
-      <c r="E133">
-        <v>474460000</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="6"/>
-      <c r="C134" s="7">
-        <v>18</v>
-      </c>
-      <c r="D134" s="5">
-        <f t="shared" si="3"/>
-        <v>479.73940000000005</v>
-      </c>
-      <c r="E134">
-        <v>479739400</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="6"/>
-      <c r="C135" s="7">
-        <v>19</v>
-      </c>
-      <c r="D135" s="5">
-        <f t="shared" si="3"/>
-        <v>480.20729999999998</v>
-      </c>
-      <c r="E135">
-        <v>480207300</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="6"/>
-      <c r="C136" s="7">
-        <v>20</v>
-      </c>
-      <c r="D136" s="5">
-        <f t="shared" si="3"/>
-        <v>476.40209999999996</v>
-      </c>
-      <c r="E136">
-        <v>476402100</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="6"/>
-      <c r="C137" s="7">
-        <v>21</v>
-      </c>
-      <c r="D137" s="5">
-        <f t="shared" si="3"/>
-        <v>475.77979999999997</v>
-      </c>
-      <c r="E137">
-        <v>475779800</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B138" s="6"/>
-      <c r="C138" s="7">
-        <v>22</v>
-      </c>
-      <c r="D138" s="5">
-        <f t="shared" si="3"/>
-        <v>481.5213</v>
-      </c>
-      <c r="E138">
-        <v>481521300</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B139" s="6"/>
-      <c r="C139" s="7">
-        <v>23</v>
-      </c>
-      <c r="D139" s="5">
-        <f t="shared" si="3"/>
-        <v>479.98990000000003</v>
-      </c>
-      <c r="E139">
-        <v>479989900</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="6"/>
-      <c r="C140" s="7">
-        <v>24</v>
-      </c>
-      <c r="D140" s="5">
-        <f t="shared" si="3"/>
-        <v>483.58340000000004</v>
-      </c>
-      <c r="E140">
-        <v>483583400</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B141" s="6"/>
-      <c r="C141" s="7">
-        <v>25</v>
-      </c>
-      <c r="D141" s="5">
-        <f t="shared" si="3"/>
-        <v>488.98359999999997</v>
-      </c>
-      <c r="E141">
-        <v>488983600</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B142" s="6"/>
-      <c r="C142" s="7">
-        <v>26</v>
-      </c>
-      <c r="D142" s="5">
-        <f t="shared" si="3"/>
-        <v>485.46290000000005</v>
-      </c>
-      <c r="E142">
-        <v>485462900</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B143" s="6"/>
-      <c r="C143" s="7">
-        <v>27</v>
-      </c>
-      <c r="D143" s="5">
-        <f t="shared" si="3"/>
-        <v>481.93079999999998</v>
-      </c>
-      <c r="E143">
-        <v>481930800</v>
-      </c>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="6"/>
-      <c r="C144" s="7">
-        <v>28</v>
-      </c>
-      <c r="D144" s="5">
-        <f t="shared" si="3"/>
-        <v>489.17720000000003</v>
-      </c>
-      <c r="E144">
-        <v>489177200</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B145" s="6"/>
-      <c r="C145" s="7">
-        <v>29</v>
-      </c>
-      <c r="D145" s="5">
-        <f t="shared" si="3"/>
-        <v>488.79950000000002</v>
-      </c>
-      <c r="E145">
-        <v>488799500</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B146" s="6"/>
-      <c r="C146" s="7">
-        <v>30</v>
-      </c>
-      <c r="D146" s="5">
-        <f t="shared" si="3"/>
-        <v>489.85950000000003</v>
-      </c>
-      <c r="E146">
-        <v>489859500</v>
-      </c>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B147" s="6"/>
-      <c r="C147" s="7">
-        <v>31</v>
-      </c>
-      <c r="D147" s="5">
-        <f t="shared" si="3"/>
-        <v>485.4529</v>
-      </c>
-      <c r="E147">
-        <v>485452900</v>
-      </c>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="8"/>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="8"/>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="8"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="8"/>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="8"/>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="8"/>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="8"/>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="8"/>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E125" s="8"/>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E126" s="8"/>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="8"/>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E128" s="8"/>
+    </row>
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E129" s="8"/>
+    </row>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E130" s="8"/>
+    </row>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E131" s="8"/>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="8"/>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E133" s="8"/>
+    </row>
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E134" s="8"/>
+    </row>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E135" s="8"/>
+    </row>
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E136" s="8"/>
+    </row>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E137" s="8"/>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E138" s="8"/>
+    </row>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E139" s="8"/>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E140" s="9"/>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E141" s="9"/>
+    </row>
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E142" s="9"/>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E143" s="9"/>
+    </row>
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E144" s="9"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E145" s="9"/>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E146" s="9"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E147" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>